<commit_message>
apports en pct reco
</commit_message>
<xml_diff>
--- a/in/reco_nut.xlsx
+++ b/in/reco_nut.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MS-nutrition-RM\kDrive\Common documents\MS-Nutrition\2. DATABASE\INCA3\inca3Analyse\in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09446B26-8B9E-458A-843D-EFA8428FFD48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8704830B-89BA-4D39-ADE8-9270F121B7F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4389" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4385" uniqueCount="245">
   <si>
     <t>Références nutritionnelles françaises pour différentes sous-populations : Enfants (3-17 ans) et Adultes</t>
   </si>
@@ -832,9 +832,6 @@
     <t>lipides_pctNRJ</t>
   </si>
   <si>
-    <t>_pctNRJ</t>
-  </si>
-  <si>
     <t>proteines_pctNRJ</t>
   </si>
   <si>
@@ -845,17 +842,27 @@
   </si>
   <si>
     <t>vitamine_b3_pctNRJ</t>
+  </si>
+  <si>
+    <t>fibres_pctNRJ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1041,50 +1048,50 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="20" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1327,74 +1334,74 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
     </row>
     <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
     <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -1559,16 +1566,16 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="26" t="s">
+      <c r="A25" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="25" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="26"/>
-      <c r="B26" s="26"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="25"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
@@ -1612,8 +1619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P106"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="80" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J3"/>
+    <sheetView topLeftCell="A25" zoomScale="80" workbookViewId="0">
+      <selection activeCell="F107" sqref="F107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1638,7 +1645,7 @@
       <c r="E1" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="25" t="s">
         <v>206</v>
       </c>
       <c r="G1" t="s">
@@ -1662,13 +1669,13 @@
       <c r="M1" t="s">
         <v>51</v>
       </c>
-      <c r="N1" s="26" t="s">
+      <c r="N1" s="25" t="s">
         <v>223</v>
       </c>
-      <c r="O1" s="26" t="s">
+      <c r="O1" s="25" t="s">
         <v>224</v>
       </c>
-      <c r="P1" s="26" t="s">
+      <c r="P1" s="25" t="s">
         <v>225</v>
       </c>
     </row>
@@ -1697,13 +1704,13 @@
       <c r="L2" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="N2" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O2" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P2" s="26" t="s">
+      <c r="N2" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O2" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P2" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -1732,13 +1739,13 @@
       <c r="L3" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="N3" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O3" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P3" s="26" t="s">
+      <c r="N3" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O3" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P3" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -1764,13 +1771,13 @@
       <c r="L4" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="N4" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O4" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P4" s="26" t="s">
+      <c r="N4" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O4" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P4" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -1796,13 +1803,13 @@
       <c r="L5" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="N5" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O5" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P5" s="26" t="s">
+      <c r="N5" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O5" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P5" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -1828,13 +1835,13 @@
       <c r="L6" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="N6" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O6" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P6" s="26" t="s">
+      <c r="N6" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O6" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P6" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -1860,13 +1867,13 @@
       <c r="L7" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="N7" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O7" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P7" s="26" t="s">
+      <c r="N7" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O7" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P7" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -1895,13 +1902,13 @@
       <c r="L8" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="N8" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O8" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P8" s="26" t="s">
+      <c r="N8" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O8" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P8" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -1930,13 +1937,13 @@
       <c r="L9" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="N9" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O9" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P9" s="26" t="s">
+      <c r="N9" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O9" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P9" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -1965,13 +1972,13 @@
       <c r="L10" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="N10" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O10" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P10" s="26" t="s">
+      <c r="N10" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O10" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P10" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2000,13 +2007,13 @@
       <c r="L11" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="N11" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O11" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P11" s="26" t="s">
+      <c r="N11" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O11" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P11" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2035,13 +2042,13 @@
       <c r="L12" s="11" t="s">
         <v>236</v>
       </c>
-      <c r="N12" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O12" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P12" s="26" t="s">
+      <c r="N12" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O12" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P12" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2070,13 +2077,13 @@
       <c r="L13" s="11" t="s">
         <v>236</v>
       </c>
-      <c r="N13" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O13" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P13" s="26" t="s">
+      <c r="N13" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O13" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P13" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2108,13 +2115,13 @@
       <c r="L14" s="11" t="s">
         <v>237</v>
       </c>
-      <c r="N14" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O14" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P14" s="26" t="s">
+      <c r="N14" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O14" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P14" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2146,13 +2153,13 @@
       <c r="L15" s="11" t="s">
         <v>237</v>
       </c>
-      <c r="N15" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O15" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P15" s="26" t="s">
+      <c r="N15" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O15" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P15" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2178,13 +2185,13 @@
       <c r="L16" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="N16" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O16" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P16" s="26" t="s">
+      <c r="N16" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O16" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P16" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2210,13 +2217,13 @@
       <c r="L17" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="N17" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O17" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P17" s="26" t="s">
+      <c r="N17" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O17" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P17" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2242,8 +2249,8 @@
       <c r="L18" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="O18" s="26"/>
-      <c r="P18" s="26"/>
+      <c r="O18" s="25"/>
+      <c r="P18" s="25"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -2290,13 +2297,13 @@
       <c r="L20" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="N20" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O20" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P20" s="26" t="s">
+      <c r="N20" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O20" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P20" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2322,13 +2329,13 @@
       <c r="L21" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="N21" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O21" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P21" s="26" t="s">
+      <c r="N21" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O21" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P21" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2360,13 +2367,13 @@
       <c r="L22" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="N22" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O22" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P22" s="26" t="s">
+      <c r="N22" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O22" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P22" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2398,13 +2405,13 @@
       <c r="L23" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="N23" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O23" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P23" s="26" t="s">
+      <c r="N23" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O23" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P23" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2436,13 +2443,13 @@
       <c r="L24" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="N24" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O24" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P24" s="26" t="s">
+      <c r="N24" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O24" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P24" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2474,13 +2481,13 @@
       <c r="L25" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="N25" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O25" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P25" s="26" t="s">
+      <c r="N25" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O25" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P25" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2541,13 +2548,13 @@
       <c r="L27" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="N27" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O27" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P27" s="26" t="s">
+      <c r="N27" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O27" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P27" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2579,9 +2586,9 @@
       <c r="L28" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="N28" s="26"/>
-      <c r="O28" s="26"/>
-      <c r="P28" s="26"/>
+      <c r="N28" s="25"/>
+      <c r="O28" s="25"/>
+      <c r="P28" s="25"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -2611,13 +2618,13 @@
       <c r="L29" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="N29" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O29" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P29" s="26" t="s">
+      <c r="N29" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O29" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P29" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2741,16 +2748,16 @@
       <c r="K34" t="s">
         <v>37</v>
       </c>
-      <c r="L34" s="26" t="s">
+      <c r="L34" s="25" t="s">
         <v>180</v>
       </c>
-      <c r="N34" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O34" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P34" s="26" t="s">
+      <c r="N34" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O34" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P34" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2776,16 +2783,16 @@
       <c r="K35" t="s">
         <v>37</v>
       </c>
-      <c r="L35" s="26" t="s">
+      <c r="L35" s="25" t="s">
         <v>180</v>
       </c>
-      <c r="N35" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O35" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P35" s="26" t="s">
+      <c r="N35" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O35" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P35" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2814,16 +2821,16 @@
       <c r="K36" t="s">
         <v>37</v>
       </c>
-      <c r="L36" s="26" t="s">
+      <c r="L36" s="25" t="s">
         <v>231</v>
       </c>
-      <c r="N36" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O36" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P36" s="26" t="s">
+      <c r="N36" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O36" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P36" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2852,16 +2859,16 @@
       <c r="K37" t="s">
         <v>37</v>
       </c>
-      <c r="L37" s="26" t="s">
+      <c r="L37" s="25" t="s">
         <v>232</v>
       </c>
-      <c r="N37" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O37" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P37" s="26" t="s">
+      <c r="N37" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O37" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P37" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2887,16 +2894,16 @@
       <c r="K38" t="s">
         <v>37</v>
       </c>
-      <c r="L38" s="26" t="s">
+      <c r="L38" s="25" t="s">
         <v>231</v>
       </c>
-      <c r="N38" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O38" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P38" s="26" t="s">
+      <c r="N38" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O38" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P38" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2922,16 +2929,16 @@
       <c r="K39" t="s">
         <v>37</v>
       </c>
-      <c r="L39" s="26" t="s">
+      <c r="L39" s="25" t="s">
         <v>182</v>
       </c>
-      <c r="N39" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O39" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P39" s="26" t="s">
+      <c r="N39" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O39" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P39" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2957,16 +2964,16 @@
       <c r="K40" t="s">
         <v>37</v>
       </c>
-      <c r="L40" s="26" t="s">
+      <c r="L40" s="25" t="s">
         <v>182</v>
       </c>
-      <c r="N40" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O40" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P40" s="26" t="s">
+      <c r="N40" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O40" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P40" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2989,16 +2996,16 @@
       <c r="K41" t="s">
         <v>37</v>
       </c>
-      <c r="L41" s="26" t="s">
+      <c r="L41" s="25" t="s">
         <v>183</v>
       </c>
-      <c r="N41" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O41" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P41" s="26" t="s">
+      <c r="N41" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O41" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P41" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3021,16 +3028,16 @@
       <c r="K42" t="s">
         <v>37</v>
       </c>
-      <c r="L42" s="26" t="s">
+      <c r="L42" s="25" t="s">
         <v>183</v>
       </c>
-      <c r="N42" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O42" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P42" s="26" t="s">
+      <c r="N42" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O42" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P42" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3053,16 +3060,16 @@
       <c r="K43" t="s">
         <v>37</v>
       </c>
-      <c r="L43" s="26" t="s">
+      <c r="L43" s="25" t="s">
         <v>184</v>
       </c>
-      <c r="N43" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O43" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P43" s="26" t="s">
+      <c r="N43" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O43" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P43" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3085,16 +3092,16 @@
       <c r="K44" t="s">
         <v>37</v>
       </c>
-      <c r="L44" s="26" t="s">
+      <c r="L44" s="25" t="s">
         <v>184</v>
       </c>
-      <c r="N44" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O44" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P44" s="26" t="s">
+      <c r="N44" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O44" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P44" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3218,16 +3225,16 @@
       <c r="K49" t="s">
         <v>37</v>
       </c>
-      <c r="L49" s="26" t="s">
+      <c r="L49" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="N49" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O49" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P49" s="26" t="s">
+      <c r="N49" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O49" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P49" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3253,16 +3260,16 @@
       <c r="K50" t="s">
         <v>37</v>
       </c>
-      <c r="L50" s="26" t="s">
+      <c r="L50" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="N50" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O50" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P50" s="26" t="s">
+      <c r="N50" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O50" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P50" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3285,16 +3292,16 @@
       <c r="K51" t="s">
         <v>37</v>
       </c>
-      <c r="L51" s="26" t="s">
+      <c r="L51" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="N51" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O51" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P51" s="26" t="s">
+      <c r="N51" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O51" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P51" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3317,16 +3324,16 @@
       <c r="K52" t="s">
         <v>37</v>
       </c>
-      <c r="L52" s="26" t="s">
+      <c r="L52" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="N52" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O52" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P52" s="26" t="s">
+      <c r="N52" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O52" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P52" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3352,16 +3359,16 @@
       <c r="K53" t="s">
         <v>37</v>
       </c>
-      <c r="L53" s="26" t="s">
+      <c r="L53" s="25" t="s">
         <v>188</v>
       </c>
-      <c r="N53" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O53" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P53" s="26" t="s">
+      <c r="N53" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O53" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P53" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3387,16 +3394,16 @@
       <c r="K54" t="s">
         <v>37</v>
       </c>
-      <c r="L54" s="26" t="s">
+      <c r="L54" s="25" t="s">
         <v>188</v>
       </c>
-      <c r="N54" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O54" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P54" s="26" t="s">
+      <c r="N54" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O54" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P54" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3428,16 +3435,16 @@
       <c r="K55" t="s">
         <v>37</v>
       </c>
-      <c r="L55" s="26" t="s">
+      <c r="L55" s="25" t="s">
         <v>228</v>
       </c>
-      <c r="N55" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O55" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P55" s="26" t="s">
+      <c r="N55" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O55" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P55" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3469,16 +3476,16 @@
       <c r="K56" t="s">
         <v>37</v>
       </c>
-      <c r="L56" s="26" t="s">
+      <c r="L56" s="25" t="s">
         <v>229</v>
       </c>
-      <c r="N56" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O56" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P56" s="26" t="s">
+      <c r="N56" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O56" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P56" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3510,16 +3517,16 @@
       <c r="K57" t="s">
         <v>37</v>
       </c>
-      <c r="L57" s="26" t="s">
+      <c r="L57" s="25" t="s">
         <v>230</v>
       </c>
-      <c r="N57" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O57" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P57" s="26" t="s">
+      <c r="N57" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O57" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P57" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3551,16 +3558,16 @@
       <c r="K58" t="s">
         <v>37</v>
       </c>
-      <c r="L58" s="26" t="s">
+      <c r="L58" s="25" t="s">
         <v>228</v>
       </c>
-      <c r="N58" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O58" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P58" s="26" t="s">
+      <c r="N58" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O58" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P58" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3592,16 +3599,16 @@
       <c r="K59" t="s">
         <v>37</v>
       </c>
-      <c r="L59" s="26" t="s">
+      <c r="L59" s="25" t="s">
         <v>229</v>
       </c>
-      <c r="N59" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O59" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P59" s="26" t="s">
+      <c r="N59" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O59" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P59" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3633,16 +3640,16 @@
       <c r="K60" t="s">
         <v>37</v>
       </c>
-      <c r="L60" s="26" t="s">
+      <c r="L60" s="25" t="s">
         <v>230</v>
       </c>
-      <c r="N60" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O60" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P60" s="26" t="s">
+      <c r="N60" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O60" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P60" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3671,19 +3678,19 @@
       <c r="K61" t="s">
         <v>26</v>
       </c>
-      <c r="L61" s="26" t="s">
-        <v>241</v>
+      <c r="L61" s="25" t="s">
+        <v>240</v>
       </c>
       <c r="M61" t="s">
         <v>97</v>
       </c>
-      <c r="N61" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O61" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P61" s="26"/>
+      <c r="N61" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O61" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P61" s="25"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
@@ -3710,15 +3717,15 @@
       <c r="K62" t="s">
         <v>99</v>
       </c>
-      <c r="L62" s="26" t="s">
-        <v>241</v>
+      <c r="L62" s="25" t="s">
+        <v>240</v>
       </c>
       <c r="M62" t="s">
         <v>100</v>
       </c>
-      <c r="N62" s="26"/>
-      <c r="O62" s="26"/>
-      <c r="P62" s="26" t="s">
+      <c r="N62" s="25"/>
+      <c r="O62" s="25"/>
+      <c r="P62" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3747,19 +3754,19 @@
       <c r="K63" t="s">
         <v>26</v>
       </c>
-      <c r="L63" s="26" t="s">
-        <v>241</v>
+      <c r="L63" s="25" t="s">
+        <v>240</v>
       </c>
       <c r="M63" t="s">
         <v>97</v>
       </c>
-      <c r="N63" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O63" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P63" s="26"/>
+      <c r="N63" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O63" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P63" s="25"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
@@ -3786,15 +3793,15 @@
       <c r="K64" t="s">
         <v>99</v>
       </c>
-      <c r="L64" s="26" t="s">
-        <v>241</v>
+      <c r="L64" s="25" t="s">
+        <v>240</v>
       </c>
       <c r="M64" t="s">
         <v>100</v>
       </c>
-      <c r="N64" s="26"/>
-      <c r="O64" s="26"/>
-      <c r="P64" s="26" t="s">
+      <c r="N64" s="25"/>
+      <c r="O64" s="25"/>
+      <c r="P64" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3818,19 +3825,19 @@
       <c r="K65" t="s">
         <v>26</v>
       </c>
-      <c r="L65" s="26" t="s">
+      <c r="L65" s="25" t="s">
         <v>227</v>
       </c>
       <c r="M65" t="s">
         <v>97</v>
       </c>
-      <c r="N65" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O65" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P65" s="26"/>
+      <c r="N65" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O65" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P65" s="25"/>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
@@ -3852,15 +3859,15 @@
       <c r="K66" t="s">
         <v>99</v>
       </c>
-      <c r="L66" s="26" t="s">
+      <c r="L66" s="25" t="s">
         <v>227</v>
       </c>
       <c r="M66" t="s">
         <v>100</v>
       </c>
-      <c r="N66" s="26"/>
-      <c r="O66" s="26"/>
-      <c r="P66" s="26" t="s">
+      <c r="N66" s="25"/>
+      <c r="O66" s="25"/>
+      <c r="P66" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3884,19 +3891,19 @@
       <c r="K67" t="s">
         <v>26</v>
       </c>
-      <c r="L67" s="26" t="s">
+      <c r="L67" s="25" t="s">
         <v>227</v>
       </c>
       <c r="M67" t="s">
         <v>97</v>
       </c>
-      <c r="N67" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O67" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P67" s="26"/>
+      <c r="N67" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O67" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P67" s="25"/>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
@@ -3918,15 +3925,15 @@
       <c r="K68" t="s">
         <v>99</v>
       </c>
-      <c r="L68" s="26" t="s">
+      <c r="L68" s="25" t="s">
         <v>227</v>
       </c>
       <c r="M68" t="s">
         <v>100</v>
       </c>
-      <c r="N68" s="26"/>
-      <c r="O68" s="26"/>
-      <c r="P68" s="26" t="s">
+      <c r="N68" s="25"/>
+      <c r="O68" s="25"/>
+      <c r="P68" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3952,8 +3959,8 @@
       <c r="M69" t="s">
         <v>75</v>
       </c>
-      <c r="N69" s="26"/>
-      <c r="O69" s="26"/>
+      <c r="N69" s="25"/>
+      <c r="O69" s="25"/>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
@@ -4000,16 +4007,16 @@
       <c r="K71" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="L71" s="26" t="s">
-        <v>242</v>
-      </c>
-      <c r="N71" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O71" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P71" s="26" t="s">
+      <c r="L71" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="N71" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O71" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P71" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4035,16 +4042,16 @@
       <c r="K72" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="L72" s="26" t="s">
-        <v>242</v>
-      </c>
-      <c r="N72" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O72" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P72" s="26" t="s">
+      <c r="L72" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="N72" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O72" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P72" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4076,13 +4083,13 @@
       <c r="L73" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="N73" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O73" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P73" s="26" t="s">
+      <c r="N73" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O73" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P73" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4114,13 +4121,13 @@
       <c r="L74" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="N74" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O74" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P74" s="26" t="s">
+      <c r="N74" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O74" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P74" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4134,11 +4141,11 @@
       <c r="D75" t="s">
         <v>105</v>
       </c>
-      <c r="E75" s="26" t="s">
+      <c r="E75" s="25" t="s">
         <v>226</v>
       </c>
-      <c r="F75" s="14" t="s">
-        <v>55</v>
+      <c r="F75" s="14">
+        <v>1</v>
       </c>
       <c r="G75">
         <v>3.0144442118484405E-4</v>
@@ -4149,16 +4156,16 @@
       <c r="K75" t="s">
         <v>37</v>
       </c>
-      <c r="L75" s="26" t="s">
-        <v>243</v>
-      </c>
-      <c r="N75" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O75" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P75" s="26" t="s">
+      <c r="L75" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="N75" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O75" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P75" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4172,11 +4179,11 @@
       <c r="D76" t="s">
         <v>105</v>
       </c>
-      <c r="E76" s="26" t="s">
+      <c r="E76" s="25" t="s">
         <v>226</v>
       </c>
-      <c r="F76" s="14" t="s">
-        <v>55</v>
+      <c r="F76" s="14">
+        <v>1</v>
       </c>
       <c r="G76">
         <v>3.0144442118484405E-4</v>
@@ -4187,16 +4194,16 @@
       <c r="K76" t="s">
         <v>37</v>
       </c>
-      <c r="L76" s="26" t="s">
-        <v>243</v>
-      </c>
-      <c r="N76" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O76" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P76" s="26" t="s">
+      <c r="L76" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="N76" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O76" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P76" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4219,16 +4226,16 @@
       <c r="K77" t="s">
         <v>37</v>
       </c>
-      <c r="L77" s="26" t="s">
+      <c r="L77" s="25" t="s">
         <v>191</v>
       </c>
-      <c r="N77" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O77" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P77" s="26" t="s">
+      <c r="N77" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O77" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P77" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4251,16 +4258,16 @@
       <c r="K78" t="s">
         <v>37</v>
       </c>
-      <c r="L78" s="26" t="s">
+      <c r="L78" s="25" t="s">
         <v>191</v>
       </c>
-      <c r="N78" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O78" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P78" s="26" t="s">
+      <c r="N78" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O78" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P78" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4286,16 +4293,16 @@
       <c r="K79" t="s">
         <v>37</v>
       </c>
-      <c r="L79" s="26" t="s">
+      <c r="L79" s="25" t="s">
         <v>192</v>
       </c>
-      <c r="N79" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O79" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P79" s="26" t="s">
+      <c r="N79" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O79" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P79" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4321,16 +4328,16 @@
       <c r="K80" t="s">
         <v>37</v>
       </c>
-      <c r="L80" s="26" t="s">
+      <c r="L80" s="25" t="s">
         <v>192</v>
       </c>
-      <c r="N80" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O80" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P80" s="26" t="s">
+      <c r="N80" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O80" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P80" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4344,11 +4351,11 @@
       <c r="D81" t="s">
         <v>108</v>
       </c>
-      <c r="E81" s="26" t="s">
+      <c r="E81" s="25" t="s">
         <v>226</v>
       </c>
-      <c r="F81" s="14" t="s">
-        <v>55</v>
+      <c r="F81" s="14">
+        <v>1</v>
       </c>
       <c r="G81">
         <v>5.4427464936152399E-3</v>
@@ -4359,16 +4366,16 @@
       <c r="K81" t="s">
         <v>37</v>
       </c>
-      <c r="L81" s="26" t="s">
-        <v>244</v>
-      </c>
-      <c r="N81" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O81" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P81" s="26" t="s">
+      <c r="L81" s="25" t="s">
+        <v>243</v>
+      </c>
+      <c r="N81" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O81" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P81" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4382,11 +4389,11 @@
       <c r="D82" t="s">
         <v>108</v>
       </c>
-      <c r="E82" s="26" t="s">
+      <c r="E82" s="25" t="s">
         <v>226</v>
       </c>
-      <c r="F82" s="14" t="s">
-        <v>55</v>
+      <c r="F82" s="14">
+        <v>1</v>
       </c>
       <c r="G82">
         <v>5.4427464936152399E-3</v>
@@ -4397,16 +4404,16 @@
       <c r="K82" t="s">
         <v>37</v>
       </c>
-      <c r="L82" s="26" t="s">
-        <v>244</v>
-      </c>
-      <c r="N82" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O82" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P82" s="26" t="s">
+      <c r="L82" s="25" t="s">
+        <v>243</v>
+      </c>
+      <c r="N82" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O82" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P82" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4432,9 +4439,9 @@
       <c r="M83" t="s">
         <v>75</v>
       </c>
-      <c r="N83" s="26"/>
-      <c r="O83" s="26"/>
-      <c r="P83" s="26"/>
+      <c r="N83" s="25"/>
+      <c r="O83" s="25"/>
+      <c r="P83" s="25"/>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
@@ -4458,9 +4465,9 @@
       <c r="M84" t="s">
         <v>75</v>
       </c>
-      <c r="N84" s="26"/>
-      <c r="O84" s="26"/>
-      <c r="P84" s="26"/>
+      <c r="N84" s="25"/>
+      <c r="O84" s="25"/>
+      <c r="P84" s="25"/>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
@@ -4527,16 +4534,16 @@
       <c r="K87" t="s">
         <v>37</v>
       </c>
-      <c r="L87" s="26" t="s">
+      <c r="L87" s="25" t="s">
         <v>193</v>
       </c>
-      <c r="N87" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O87" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P87" s="26" t="s">
+      <c r="N87" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O87" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P87" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4559,16 +4566,16 @@
       <c r="K88" t="s">
         <v>37</v>
       </c>
-      <c r="L88" s="26" t="s">
+      <c r="L88" s="25" t="s">
         <v>193</v>
       </c>
-      <c r="N88" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O88" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P88" s="26" t="s">
+      <c r="N88" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O88" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P88" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4597,16 +4604,16 @@
       <c r="K89" t="s">
         <v>37</v>
       </c>
-      <c r="L89" s="26" t="s">
+      <c r="L89" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="N89" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O89" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P89" s="26" t="s">
+      <c r="N89" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O89" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P89" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4635,16 +4642,16 @@
       <c r="K90" t="s">
         <v>37</v>
       </c>
-      <c r="L90" s="26" t="s">
+      <c r="L90" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="N90" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O90" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P90" s="26" t="s">
+      <c r="N90" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O90" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P90" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4716,16 +4723,16 @@
       <c r="K93" t="s">
         <v>37</v>
       </c>
-      <c r="L93" s="26" t="s">
+      <c r="L93" s="25" t="s">
         <v>195</v>
       </c>
-      <c r="N93" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O93" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P93" s="26" t="s">
+      <c r="N93" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O93" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P93" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4751,16 +4758,16 @@
       <c r="K94" t="s">
         <v>37</v>
       </c>
-      <c r="L94" s="26" t="s">
+      <c r="L94" s="25" t="s">
         <v>195</v>
       </c>
-      <c r="N94" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O94" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P94" s="26" t="s">
+      <c r="N94" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O94" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P94" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4832,16 +4839,16 @@
       <c r="K97" t="s">
         <v>37</v>
       </c>
-      <c r="L97" s="26" t="s">
+      <c r="L97" s="25" t="s">
         <v>196</v>
       </c>
-      <c r="N97" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O97" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P97" s="26" t="s">
+      <c r="N97" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O97" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P97" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4867,16 +4874,16 @@
       <c r="K98" t="s">
         <v>37</v>
       </c>
-      <c r="L98" s="26" t="s">
+      <c r="L98" s="25" t="s">
         <v>196</v>
       </c>
-      <c r="N98" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O98" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P98" s="26" t="s">
+      <c r="N98" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O98" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P98" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4902,16 +4909,16 @@
       <c r="K99" t="s">
         <v>37</v>
       </c>
-      <c r="L99" s="26" t="s">
+      <c r="L99" s="25" t="s">
         <v>197</v>
       </c>
-      <c r="N99" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O99" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P99" s="26" t="s">
+      <c r="N99" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O99" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P99" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4937,16 +4944,16 @@
       <c r="K100" t="s">
         <v>37</v>
       </c>
-      <c r="L100" s="26" t="s">
+      <c r="L100" s="25" t="s">
         <v>197</v>
       </c>
-      <c r="N100" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O100" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P100" s="26" t="s">
+      <c r="N100" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O100" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P100" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4969,16 +4976,16 @@
       <c r="K101" t="s">
         <v>37</v>
       </c>
-      <c r="L101" s="26" t="s">
+      <c r="L101" s="25" t="s">
         <v>198</v>
       </c>
-      <c r="N101" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O101" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P101" s="26" t="s">
+      <c r="N101" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O101" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P101" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -5001,16 +5008,16 @@
       <c r="K102" t="s">
         <v>37</v>
       </c>
-      <c r="L102" s="26" t="s">
+      <c r="L102" s="25" t="s">
         <v>198</v>
       </c>
-      <c r="N102" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="O102" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="P102" s="26" t="s">
+      <c r="N102" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O102" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P102" s="25" t="s">
         <v>173</v>
       </c>
     </row>
@@ -5118,11 +5125,11 @@
   <dimension ref="A1:S507"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E296" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E50" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D1" sqref="D1:D1048576"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K60" sqref="K60:K77"/>
+      <selection pane="bottomRight" activeCell="M59" sqref="M59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6713,7 +6720,7 @@
         <v>203</v>
       </c>
       <c r="M58" s="11" t="s">
-        <v>177</v>
+        <v>244</v>
       </c>
       <c r="N58" s="14" t="s">
         <v>205</v>
@@ -6757,7 +6764,7 @@
         <v>203</v>
       </c>
       <c r="M59" s="11" t="s">
-        <v>177</v>
+        <v>244</v>
       </c>
       <c r="N59" s="14" t="s">
         <v>205</v>
@@ -7227,7 +7234,7 @@
         <v>22</v>
       </c>
       <c r="M72" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="N72" s="10" t="s">
         <v>199</v>
@@ -8936,7 +8943,7 @@
       <c r="L136" t="s">
         <v>37</v>
       </c>
-      <c r="M136" s="26" t="s">
+      <c r="M136" s="25" t="s">
         <v>231</v>
       </c>
     </row>
@@ -8962,7 +8969,7 @@
       <c r="L137" t="s">
         <v>37</v>
       </c>
-      <c r="M137" s="26" t="s">
+      <c r="M137" s="25" t="s">
         <v>231</v>
       </c>
     </row>
@@ -8988,7 +8995,7 @@
       <c r="L138" t="s">
         <v>37</v>
       </c>
-      <c r="M138" s="26" t="s">
+      <c r="M138" s="25" t="s">
         <v>231</v>
       </c>
       <c r="O138" s="22" t="s">
@@ -9017,7 +9024,7 @@
       <c r="L139" t="s">
         <v>37</v>
       </c>
-      <c r="M139" s="26" t="s">
+      <c r="M139" s="25" t="s">
         <v>231</v>
       </c>
       <c r="O139" s="22" t="s">
@@ -9046,7 +9053,7 @@
       <c r="L140" t="s">
         <v>37</v>
       </c>
-      <c r="M140" s="26" t="s">
+      <c r="M140" s="25" t="s">
         <v>231</v>
       </c>
       <c r="P140" s="22" t="s">
@@ -9075,7 +9082,7 @@
       <c r="L141" t="s">
         <v>37</v>
       </c>
-      <c r="M141" s="26" t="s">
+      <c r="M141" s="25" t="s">
         <v>231</v>
       </c>
       <c r="P141" s="22" t="s">
@@ -9104,7 +9111,7 @@
       <c r="L142" t="s">
         <v>37</v>
       </c>
-      <c r="M142" s="26" t="s">
+      <c r="M142" s="25" t="s">
         <v>231</v>
       </c>
       <c r="Q142" s="22" t="s">
@@ -9133,7 +9140,7 @@
       <c r="L143" t="s">
         <v>37</v>
       </c>
-      <c r="M143" s="26" t="s">
+      <c r="M143" s="25" t="s">
         <v>231</v>
       </c>
       <c r="Q143" s="22" t="s">
@@ -9165,7 +9172,7 @@
       <c r="L144" t="s">
         <v>37</v>
       </c>
-      <c r="M144" s="26" t="s">
+      <c r="M144" s="25" t="s">
         <v>231</v>
       </c>
       <c r="R144" s="22" t="s">
@@ -9200,7 +9207,7 @@
       <c r="L145" t="s">
         <v>37</v>
       </c>
-      <c r="M145" s="26" t="s">
+      <c r="M145" s="25" t="s">
         <v>232</v>
       </c>
       <c r="R145" s="22" t="s">
@@ -9232,7 +9239,7 @@
       <c r="L146" t="s">
         <v>37</v>
       </c>
-      <c r="M146" s="26" t="s">
+      <c r="M146" s="25" t="s">
         <v>231</v>
       </c>
       <c r="R146" s="22" t="s">
@@ -12668,7 +12675,7 @@
       <c r="L274" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="M274" s="26" t="s">
+      <c r="M274" s="25" t="s">
         <v>227</v>
       </c>
       <c r="N274" s="15"/>
@@ -12707,7 +12714,7 @@
       <c r="L275" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="M275" s="26" t="s">
+      <c r="M275" s="25" t="s">
         <v>227</v>
       </c>
       <c r="N275" s="15"/>
@@ -12746,7 +12753,7 @@
       <c r="L276" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="M276" s="26" t="s">
+      <c r="M276" s="25" t="s">
         <v>227</v>
       </c>
       <c r="N276" s="15"/>
@@ -12785,7 +12792,7 @@
       <c r="L277" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="M277" s="26" t="s">
+      <c r="M277" s="25" t="s">
         <v>227</v>
       </c>
       <c r="N277" s="15"/>
@@ -12824,7 +12831,7 @@
       <c r="L278" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="M278" s="26" t="s">
+      <c r="M278" s="25" t="s">
         <v>227</v>
       </c>
       <c r="N278" s="15"/>
@@ -12863,7 +12870,7 @@
       <c r="L279" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="M279" s="26" t="s">
+      <c r="M279" s="25" t="s">
         <v>227</v>
       </c>
       <c r="N279" s="15"/>
@@ -12902,7 +12909,7 @@
       <c r="L280" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="M280" s="26" t="s">
+      <c r="M280" s="25" t="s">
         <v>227</v>
       </c>
       <c r="N280" s="15"/>
@@ -12941,7 +12948,7 @@
       <c r="L281" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="M281" s="26" t="s">
+      <c r="M281" s="25" t="s">
         <v>227</v>
       </c>
       <c r="N281" s="15"/>
@@ -12980,7 +12987,7 @@
       <c r="L282" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="M282" s="26" t="s">
+      <c r="M282" s="25" t="s">
         <v>227</v>
       </c>
       <c r="N282" s="15"/>
@@ -13019,7 +13026,7 @@
       <c r="L283" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="M283" s="26" t="s">
+      <c r="M283" s="25" t="s">
         <v>227</v>
       </c>
       <c r="N283" s="15"/>
@@ -13056,8 +13063,8 @@
       <c r="L284" t="s">
         <v>26</v>
       </c>
-      <c r="M284" s="26" t="s">
-        <v>241</v>
+      <c r="M284" s="25" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="285" spans="1:19" x14ac:dyDescent="0.25">
@@ -13085,8 +13092,8 @@
       <c r="L285" t="s">
         <v>26</v>
       </c>
-      <c r="M285" s="26" t="s">
-        <v>241</v>
+      <c r="M285" s="25" t="s">
+        <v>240</v>
       </c>
       <c r="O285" t="s">
         <v>173</v>
@@ -13120,8 +13127,8 @@
       <c r="L286" t="s">
         <v>26</v>
       </c>
-      <c r="M286" s="26" t="s">
-        <v>241</v>
+      <c r="M286" s="25" t="s">
+        <v>240</v>
       </c>
       <c r="Q286" t="s">
         <v>173</v>
@@ -13152,8 +13159,8 @@
       <c r="L287" t="s">
         <v>26</v>
       </c>
-      <c r="M287" s="26" t="s">
-        <v>241</v>
+      <c r="M287" s="25" t="s">
+        <v>240</v>
       </c>
       <c r="R287" t="s">
         <v>173</v>
@@ -13184,8 +13191,8 @@
       <c r="L288" t="s">
         <v>26</v>
       </c>
-      <c r="M288" s="26" t="s">
-        <v>241</v>
+      <c r="M288" s="25" t="s">
+        <v>240</v>
       </c>
       <c r="S288" t="s">
         <v>173</v>
@@ -13216,8 +13223,8 @@
       <c r="L289" t="s">
         <v>26</v>
       </c>
-      <c r="M289" s="26" t="s">
-        <v>241</v>
+      <c r="M289" s="25" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="290" spans="1:19" x14ac:dyDescent="0.25">
@@ -13245,8 +13252,8 @@
       <c r="L290" t="s">
         <v>26</v>
       </c>
-      <c r="M290" s="26" t="s">
-        <v>241</v>
+      <c r="M290" s="25" t="s">
+        <v>240</v>
       </c>
       <c r="O290" t="s">
         <v>173</v>
@@ -13280,8 +13287,8 @@
       <c r="L291" t="s">
         <v>26</v>
       </c>
-      <c r="M291" s="26" t="s">
-        <v>241</v>
+      <c r="M291" s="25" t="s">
+        <v>240</v>
       </c>
       <c r="Q291" t="s">
         <v>173</v>
@@ -13312,8 +13319,8 @@
       <c r="L292" t="s">
         <v>26</v>
       </c>
-      <c r="M292" s="26" t="s">
-        <v>241</v>
+      <c r="M292" s="25" t="s">
+        <v>240</v>
       </c>
       <c r="R292" t="s">
         <v>173</v>
@@ -13344,8 +13351,8 @@
       <c r="L293" t="s">
         <v>26</v>
       </c>
-      <c r="M293" s="26" t="s">
-        <v>241</v>
+      <c r="M293" s="25" t="s">
+        <v>240</v>
       </c>
       <c r="S293" t="s">
         <v>173</v>
@@ -13413,8 +13420,8 @@
       <c r="L296" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="M296" s="26" t="s">
-        <v>242</v>
+      <c r="M296" s="25" t="s">
+        <v>241</v>
       </c>
       <c r="O296" s="14" t="s">
         <v>173</v>
@@ -13454,8 +13461,8 @@
       <c r="L297" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="M297" s="26" t="s">
-        <v>242</v>
+      <c r="M297" s="25" t="s">
+        <v>241</v>
       </c>
       <c r="O297" s="14" t="s">
         <v>173</v>
@@ -13963,8 +13970,8 @@
       <c r="L314" t="s">
         <v>37</v>
       </c>
-      <c r="M314" s="26" t="s">
-        <v>243</v>
+      <c r="M314" s="25" t="s">
+        <v>242</v>
       </c>
       <c r="O314" s="23" t="s">
         <v>173</v>
@@ -14008,8 +14015,8 @@
       <c r="L315" t="s">
         <v>37</v>
       </c>
-      <c r="M315" s="26" t="s">
-        <v>243</v>
+      <c r="M315" s="25" t="s">
+        <v>242</v>
       </c>
       <c r="O315" s="23" t="s">
         <v>173</v>
@@ -14832,8 +14839,8 @@
       <c r="L346" t="s">
         <v>37</v>
       </c>
-      <c r="M346" s="26" t="s">
-        <v>244</v>
+      <c r="M346" s="25" t="s">
+        <v>243</v>
       </c>
       <c r="O346" s="10" t="s">
         <v>173</v>
@@ -14876,8 +14883,8 @@
       <c r="L347" t="s">
         <v>37</v>
       </c>
-      <c r="M347" s="26" t="s">
-        <v>244</v>
+      <c r="M347" s="25" t="s">
+        <v>243</v>
       </c>
       <c r="O347" s="10" t="s">
         <v>173</v>
@@ -18859,7 +18866,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:S507" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
-  <phoneticPr fontId="21" type="noConversion"/>
+  <phoneticPr fontId="22" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>

</xml_diff>

<commit_message>
finalisation mar mer pour tous els individus et PNNS
</commit_message>
<xml_diff>
--- a/in/reco_nut.xlsx
+++ b/in/reco_nut.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MS-nutrition-RM\kDrive\Common documents\MS-Nutrition\2. DATABASE\INCA3\inca3Analyse\in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4B1294-6E93-4115-98D1-40328A4B7DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C727C5F-B58D-4F8D-A382-144655BAD799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="READme" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="REFERENCES" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ADULTES!$A$1:$M$106</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ADULTES!$A$1:$M$108</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ENFANTS!$A$1:$S$507</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4385" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4413" uniqueCount="245">
   <si>
     <t>Références nutritionnelles françaises pour différentes sous-populations : Enfants (3-17 ans) et Adultes</t>
   </si>
@@ -751,9 +751,6 @@
     <t>15 % abs non heminique 25% heminique - traduire le besoin selon l'équation en fct poids corporel</t>
   </si>
   <si>
-    <t>Pas de précision si la valeur adulte s'applique pour les enfants - voir a posteriori</t>
-  </si>
-  <si>
     <t>[7:11[</t>
   </si>
   <si>
@@ -845,17 +842,27 @@
   </si>
   <si>
     <t>fibres_pctNRJ</t>
+  </si>
+  <si>
+    <t>Pas de précision si la valeur adulte s'applique pour les enfants - voir a posteriori NON officiel !! Pr le MER</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1048,50 +1055,52 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="20" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1334,74 +1343,74 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
     </row>
     <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
     <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -1567,10 +1576,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="B25" s="25" t="s">
         <v>221</v>
-      </c>
-      <c r="B25" s="25" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1617,10 +1626,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P106"/>
+  <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56:I56"/>
+    <sheetView zoomScale="80" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1670,13 +1679,13 @@
         <v>51</v>
       </c>
       <c r="N1" s="25" t="s">
+        <v>222</v>
+      </c>
+      <c r="O1" s="25" t="s">
         <v>223</v>
       </c>
-      <c r="O1" s="25" t="s">
+      <c r="P1" s="25" t="s">
         <v>224</v>
-      </c>
-      <c r="P1" s="25" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -1702,7 +1711,7 @@
         <v>22</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="N2" s="25" t="s">
         <v>173</v>
@@ -1737,7 +1746,7 @@
         <v>22</v>
       </c>
       <c r="L3" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="N3" s="25" t="s">
         <v>173</v>
@@ -1833,7 +1842,7 @@
         <v>22</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N6" s="25" t="s">
         <v>173</v>
@@ -1865,7 +1874,7 @@
         <v>22</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N7" s="25" t="s">
         <v>173</v>
@@ -1884,23 +1893,20 @@
       <c r="B8" t="s">
         <v>53</v>
       </c>
-      <c r="D8" t="s">
-        <v>60</v>
+      <c r="D8" s="26" t="s">
+        <v>127</v>
       </c>
       <c r="E8" t="s">
-        <v>55</v>
-      </c>
-      <c r="F8">
-        <v>9</v>
-      </c>
-      <c r="J8">
-        <v>8</v>
+        <v>58</v>
+      </c>
+      <c r="I8">
+        <v>500</v>
       </c>
       <c r="K8" t="s">
         <v>22</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
       <c r="N8" s="25" t="s">
         <v>173</v>
@@ -1919,23 +1925,20 @@
       <c r="B9" t="s">
         <v>53</v>
       </c>
-      <c r="D9" t="s">
-        <v>60</v>
+      <c r="D9" s="26" t="s">
+        <v>127</v>
       </c>
       <c r="E9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9">
-        <v>9</v>
-      </c>
-      <c r="J9">
-        <v>8</v>
+        <v>58</v>
+      </c>
+      <c r="I9">
+        <v>500</v>
       </c>
       <c r="K9" t="s">
         <v>22</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
       <c r="N9" s="25" t="s">
         <v>173</v>
@@ -1955,7 +1958,7 @@
         <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E10" t="s">
         <v>55</v>
@@ -1963,14 +1966,14 @@
       <c r="F10">
         <v>9</v>
       </c>
-      <c r="I10">
-        <v>4</v>
+      <c r="J10">
+        <v>8</v>
       </c>
       <c r="K10" t="s">
         <v>22</v>
       </c>
       <c r="L10" s="11" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="N10" s="25" t="s">
         <v>173</v>
@@ -1990,7 +1993,7 @@
         <v>53</v>
       </c>
       <c r="D11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E11" t="s">
         <v>55</v>
@@ -1998,14 +2001,14 @@
       <c r="F11">
         <v>9</v>
       </c>
-      <c r="I11">
-        <v>4</v>
+      <c r="J11">
+        <v>8</v>
       </c>
       <c r="K11" t="s">
         <v>22</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="N11" s="25" t="s">
         <v>173</v>
@@ -2025,7 +2028,7 @@
         <v>53</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E12" t="s">
         <v>55</v>
@@ -2034,13 +2037,13 @@
         <v>9</v>
       </c>
       <c r="I12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K12" t="s">
         <v>22</v>
       </c>
       <c r="L12" s="11" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="N12" s="25" t="s">
         <v>173</v>
@@ -2060,7 +2063,7 @@
         <v>53</v>
       </c>
       <c r="D13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E13" t="s">
         <v>55</v>
@@ -2069,13 +2072,13 @@
         <v>9</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K13" t="s">
         <v>22</v>
       </c>
       <c r="L13" s="11" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="N13" s="25" t="s">
         <v>173</v>
@@ -2095,7 +2098,7 @@
         <v>53</v>
       </c>
       <c r="D14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E14" t="s">
         <v>55</v>
@@ -2104,16 +2107,13 @@
         <v>9</v>
       </c>
       <c r="I14">
-        <v>15</v>
-      </c>
-      <c r="J14">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="K14" t="s">
         <v>22</v>
       </c>
       <c r="L14" s="11" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="N14" s="25" t="s">
         <v>173</v>
@@ -2133,7 +2133,7 @@
         <v>53</v>
       </c>
       <c r="D15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E15" t="s">
         <v>55</v>
@@ -2142,16 +2142,13 @@
         <v>9</v>
       </c>
       <c r="I15">
-        <v>15</v>
-      </c>
-      <c r="J15">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="K15" t="s">
         <v>22</v>
       </c>
       <c r="L15" s="11" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="N15" s="25" t="s">
         <v>173</v>
@@ -2171,19 +2168,25 @@
         <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E16" t="s">
-        <v>65</v>
+        <v>55</v>
+      </c>
+      <c r="F16">
+        <v>9</v>
       </c>
       <c r="I16">
-        <v>2000</v>
+        <v>15</v>
+      </c>
+      <c r="J16">
+        <v>20</v>
       </c>
       <c r="K16" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="L16" s="11" t="s">
-        <v>176</v>
+        <v>236</v>
       </c>
       <c r="N16" s="25" t="s">
         <v>173</v>
@@ -2203,19 +2206,25 @@
         <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E17" t="s">
-        <v>65</v>
+        <v>55</v>
+      </c>
+      <c r="F17">
+        <v>9</v>
       </c>
       <c r="I17">
-        <v>2500</v>
+        <v>15</v>
+      </c>
+      <c r="J17">
+        <v>20</v>
       </c>
       <c r="K17" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="L17" s="11" t="s">
-        <v>176</v>
+        <v>236</v>
       </c>
       <c r="N17" s="25" t="s">
         <v>173</v>
@@ -2235,22 +2244,29 @@
         <v>53</v>
       </c>
       <c r="D18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I18">
-        <v>2100</v>
+        <v>2000</v>
       </c>
       <c r="K18" t="s">
         <v>26</v>
       </c>
       <c r="L18" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="O18" s="25"/>
-      <c r="P18" s="25"/>
+        <v>176</v>
+      </c>
+      <c r="N18" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O18" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P18" s="25" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -2260,19 +2276,28 @@
         <v>53</v>
       </c>
       <c r="D19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I19">
-        <v>2600</v>
+        <v>2500</v>
       </c>
       <c r="K19" t="s">
         <v>26</v>
       </c>
       <c r="L19" s="11" t="s">
-        <v>178</v>
+        <v>176</v>
+      </c>
+      <c r="N19" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O19" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P19" s="25" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -2283,29 +2308,22 @@
         <v>53</v>
       </c>
       <c r="D20" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E20" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="I20">
-        <v>30</v>
+        <v>2100</v>
       </c>
       <c r="K20" t="s">
         <v>26</v>
       </c>
       <c r="L20" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="N20" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="O20" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="P20" s="25" t="s">
-        <v>173</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="O20" s="25"/>
+      <c r="P20" s="25"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -2315,28 +2333,19 @@
         <v>53</v>
       </c>
       <c r="D21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E21" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="I21">
-        <v>30</v>
+        <v>2600</v>
       </c>
       <c r="K21" t="s">
         <v>26</v>
       </c>
       <c r="L21" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="N21" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="O21" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="P21" s="25" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -2347,25 +2356,19 @@
         <v>53</v>
       </c>
       <c r="D22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E22" t="s">
-        <v>55</v>
-      </c>
-      <c r="F22">
-        <v>4</v>
+        <v>65</v>
       </c>
       <c r="I22">
-        <v>40</v>
-      </c>
-      <c r="J22">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="K22" t="s">
         <v>26</v>
       </c>
       <c r="L22" s="11" t="s">
-        <v>238</v>
+        <v>177</v>
       </c>
       <c r="N22" s="25" t="s">
         <v>173</v>
@@ -2385,25 +2388,19 @@
         <v>53</v>
       </c>
       <c r="D23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E23" t="s">
-        <v>55</v>
-      </c>
-      <c r="F23">
-        <v>4</v>
+        <v>65</v>
       </c>
       <c r="I23">
-        <v>40</v>
-      </c>
-      <c r="J23">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="K23" t="s">
         <v>26</v>
       </c>
       <c r="L23" s="11" t="s">
-        <v>238</v>
+        <v>177</v>
       </c>
       <c r="N23" s="25" t="s">
         <v>173</v>
@@ -2423,25 +2420,25 @@
         <v>53</v>
       </c>
       <c r="D24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E24" t="s">
         <v>55</v>
       </c>
       <c r="F24">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="I24">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="J24">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="K24" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="L24" s="11" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="N24" s="25" t="s">
         <v>173</v>
@@ -2461,25 +2458,25 @@
         <v>53</v>
       </c>
       <c r="D25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E25" t="s">
         <v>55</v>
       </c>
       <c r="F25">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="I25">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="J25">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="K25" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="L25" s="11" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="N25" s="25" t="s">
         <v>173</v>
@@ -2496,57 +2493,66 @@
         <v>52</v>
       </c>
       <c r="B26" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="D26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E26" t="s">
-        <v>58</v>
-      </c>
-      <c r="G26">
-        <v>860</v>
-      </c>
-      <c r="H26">
-        <v>1000</v>
+        <v>55</v>
+      </c>
+      <c r="F26">
+        <v>9</v>
+      </c>
+      <c r="I26">
+        <v>35</v>
       </c>
       <c r="J26">
-        <v>2500</v>
+        <v>40</v>
       </c>
       <c r="K26" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="L26" s="11" t="s">
-        <v>179</v>
+        <v>238</v>
+      </c>
+      <c r="N26" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O26" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P26" s="25" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="D27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E27" t="s">
-        <v>58</v>
-      </c>
-      <c r="G27">
-        <v>750</v>
-      </c>
-      <c r="H27">
-        <v>950</v>
+        <v>55</v>
+      </c>
+      <c r="F27">
+        <v>9</v>
+      </c>
+      <c r="I27">
+        <v>35</v>
       </c>
       <c r="J27">
-        <v>2500</v>
+        <v>40</v>
       </c>
       <c r="K27" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="L27" s="11" t="s">
-        <v>179</v>
+        <v>238</v>
       </c>
       <c r="N27" s="25" t="s">
         <v>173</v>
@@ -2560,7 +2566,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B28" t="s">
         <v>71</v>
@@ -2586,13 +2592,10 @@
       <c r="L28" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="N28" s="25"/>
-      <c r="O28" s="25"/>
-      <c r="P28" s="25"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B29" t="s">
         <v>73</v>
@@ -2630,54 +2633,72 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B30" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="D30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E30" t="s">
         <v>58</v>
       </c>
-      <c r="I30">
-        <v>2.9</v>
+      <c r="G30">
+        <v>860</v>
+      </c>
+      <c r="H30">
+        <v>1000</v>
       </c>
       <c r="J30">
-        <v>7</v>
+        <v>2500</v>
       </c>
       <c r="K30" t="s">
         <v>37</v>
       </c>
-      <c r="M30" t="s">
-        <v>75</v>
-      </c>
+      <c r="L30" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="N30" s="25"/>
+      <c r="O30" s="25"/>
+      <c r="P30" s="25"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>56</v>
       </c>
       <c r="B31" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="D31" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E31" t="s">
         <v>58</v>
       </c>
-      <c r="I31">
-        <v>3.4</v>
+      <c r="G31">
+        <v>750</v>
+      </c>
+      <c r="H31">
+        <v>950</v>
       </c>
       <c r="J31">
-        <v>7</v>
+        <v>2500</v>
       </c>
       <c r="K31" t="s">
         <v>37</v>
       </c>
-      <c r="M31" t="s">
-        <v>75</v>
+      <c r="L31" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="N31" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O31" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P31" s="25" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -2688,13 +2709,16 @@
         <v>53</v>
       </c>
       <c r="D32" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E32" t="s">
         <v>58</v>
       </c>
       <c r="I32">
-        <v>2300</v>
+        <v>2.9</v>
+      </c>
+      <c r="J32">
+        <v>7</v>
       </c>
       <c r="K32" t="s">
         <v>37</v>
@@ -2711,13 +2735,16 @@
         <v>53</v>
       </c>
       <c r="D33" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E33" t="s">
         <v>58</v>
       </c>
       <c r="I33">
-        <v>2300</v>
+        <v>3.4</v>
+      </c>
+      <c r="J33">
+        <v>7</v>
       </c>
       <c r="K33" t="s">
         <v>37</v>
@@ -2734,31 +2761,19 @@
         <v>53</v>
       </c>
       <c r="D34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E34" t="s">
         <v>58</v>
       </c>
       <c r="I34">
-        <v>1.5</v>
-      </c>
-      <c r="J34">
-        <v>5</v>
+        <v>2300</v>
       </c>
       <c r="K34" t="s">
         <v>37</v>
       </c>
-      <c r="L34" s="25" t="s">
-        <v>180</v>
-      </c>
-      <c r="N34" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="O34" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="P34" s="25" t="s">
-        <v>173</v>
+      <c r="M34" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -2769,31 +2784,19 @@
         <v>53</v>
       </c>
       <c r="D35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E35" t="s">
         <v>58</v>
       </c>
       <c r="I35">
-        <v>1.9</v>
-      </c>
-      <c r="J35">
-        <v>5</v>
+        <v>2300</v>
       </c>
       <c r="K35" t="s">
         <v>37</v>
       </c>
-      <c r="L35" s="25" t="s">
-        <v>180</v>
-      </c>
-      <c r="N35" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="O35" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="P35" s="25" t="s">
-        <v>173</v>
+      <c r="M35" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
@@ -2803,26 +2806,23 @@
       <c r="B36" t="s">
         <v>53</v>
       </c>
-      <c r="C36" t="s">
-        <v>78</v>
-      </c>
       <c r="D36" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E36" t="s">
         <v>58</v>
       </c>
-      <c r="G36">
-        <v>7</v>
-      </c>
-      <c r="H36">
-        <v>11</v>
+      <c r="I36">
+        <v>1.5</v>
+      </c>
+      <c r="J36">
+        <v>5</v>
       </c>
       <c r="K36" t="s">
         <v>37</v>
       </c>
       <c r="L36" s="25" t="s">
-        <v>231</v>
+        <v>180</v>
       </c>
       <c r="N36" s="25" t="s">
         <v>173</v>
@@ -2836,31 +2836,28 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B37" t="s">
         <v>53</v>
       </c>
-      <c r="C37" t="s">
-        <v>80</v>
-      </c>
       <c r="D37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E37" t="s">
         <v>58</v>
       </c>
-      <c r="G37">
-        <v>7</v>
-      </c>
-      <c r="H37">
-        <v>16</v>
+      <c r="I37">
+        <v>1.9</v>
+      </c>
+      <c r="J37">
+        <v>5</v>
       </c>
       <c r="K37" t="s">
         <v>37</v>
       </c>
       <c r="L37" s="25" t="s">
-        <v>232</v>
+        <v>180</v>
       </c>
       <c r="N37" s="25" t="s">
         <v>173</v>
@@ -2874,11 +2871,14 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B38" t="s">
         <v>53</v>
       </c>
+      <c r="C38" t="s">
+        <v>78</v>
+      </c>
       <c r="D38" t="s">
         <v>79</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>58</v>
       </c>
       <c r="G38">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H38">
         <v>11</v>
@@ -2895,7 +2895,7 @@
         <v>37</v>
       </c>
       <c r="L38" s="25" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="N38" s="25" t="s">
         <v>173</v>
@@ -2914,23 +2914,26 @@
       <c r="B39" t="s">
         <v>53</v>
       </c>
+      <c r="C39" t="s">
+        <v>80</v>
+      </c>
       <c r="D39" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E39" t="s">
-        <v>82</v>
-      </c>
-      <c r="I39">
-        <v>150</v>
-      </c>
-      <c r="J39">
-        <v>600</v>
+        <v>58</v>
+      </c>
+      <c r="G39">
+        <v>7</v>
+      </c>
+      <c r="H39">
+        <v>16</v>
       </c>
       <c r="K39" t="s">
         <v>37</v>
       </c>
       <c r="L39" s="25" t="s">
-        <v>182</v>
+        <v>231</v>
       </c>
       <c r="N39" s="25" t="s">
         <v>173</v>
@@ -2950,22 +2953,22 @@
         <v>53</v>
       </c>
       <c r="D40" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E40" t="s">
-        <v>82</v>
-      </c>
-      <c r="I40">
-        <v>150</v>
-      </c>
-      <c r="J40">
-        <v>600</v>
+        <v>58</v>
+      </c>
+      <c r="G40">
+        <v>6</v>
+      </c>
+      <c r="H40">
+        <v>11</v>
       </c>
       <c r="K40" t="s">
         <v>37</v>
       </c>
       <c r="L40" s="25" t="s">
-        <v>182</v>
+        <v>230</v>
       </c>
       <c r="N40" s="25" t="s">
         <v>173</v>
@@ -2985,19 +2988,22 @@
         <v>53</v>
       </c>
       <c r="D41" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E41" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="I41">
-        <v>3500</v>
+        <v>150</v>
+      </c>
+      <c r="J41">
+        <v>600</v>
       </c>
       <c r="K41" t="s">
         <v>37</v>
       </c>
       <c r="L41" s="25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N41" s="25" t="s">
         <v>173</v>
@@ -3017,19 +3023,22 @@
         <v>53</v>
       </c>
       <c r="D42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E42" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="I42">
-        <v>3500</v>
+        <v>150</v>
+      </c>
+      <c r="J42">
+        <v>600</v>
       </c>
       <c r="K42" t="s">
         <v>37</v>
       </c>
       <c r="L42" s="25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N42" s="25" t="s">
         <v>173</v>
@@ -3049,19 +3058,19 @@
         <v>53</v>
       </c>
       <c r="D43" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E43" t="s">
         <v>58</v>
       </c>
       <c r="I43">
-        <v>300</v>
+        <v>3500</v>
       </c>
       <c r="K43" t="s">
         <v>37</v>
       </c>
       <c r="L43" s="25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N43" s="25" t="s">
         <v>173</v>
@@ -3081,19 +3090,19 @@
         <v>53</v>
       </c>
       <c r="D44" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E44" t="s">
         <v>58</v>
       </c>
       <c r="I44">
-        <v>380</v>
+        <v>3500</v>
       </c>
       <c r="K44" t="s">
         <v>37</v>
       </c>
       <c r="L44" s="25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N44" s="25" t="s">
         <v>173</v>
@@ -3113,19 +3122,28 @@
         <v>53</v>
       </c>
       <c r="D45" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E45" t="s">
         <v>58</v>
       </c>
-      <c r="J45">
-        <v>250</v>
+      <c r="I45">
+        <v>300</v>
       </c>
       <c r="K45" t="s">
         <v>37</v>
       </c>
-      <c r="M45" t="s">
-        <v>86</v>
+      <c r="L45" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="N45" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O45" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P45" s="25" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -3136,19 +3154,28 @@
         <v>53</v>
       </c>
       <c r="D46" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E46" t="s">
         <v>58</v>
       </c>
-      <c r="J46">
-        <v>250</v>
+      <c r="I46">
+        <v>380</v>
       </c>
       <c r="K46" t="s">
         <v>37</v>
       </c>
-      <c r="M46" t="s">
-        <v>86</v>
+      <c r="L46" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="N46" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O46" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P46" s="25" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
@@ -3159,22 +3186,19 @@
         <v>53</v>
       </c>
       <c r="D47" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E47" t="s">
-        <v>82</v>
-      </c>
-      <c r="I47">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="J47">
-        <v>600</v>
+        <v>250</v>
       </c>
       <c r="K47" t="s">
         <v>37</v>
       </c>
       <c r="M47" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -3185,22 +3209,19 @@
         <v>53</v>
       </c>
       <c r="D48" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E48" t="s">
-        <v>82</v>
-      </c>
-      <c r="I48">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="J48">
-        <v>600</v>
+        <v>250</v>
       </c>
       <c r="K48" t="s">
         <v>37</v>
       </c>
       <c r="M48" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
@@ -3211,31 +3232,22 @@
         <v>53</v>
       </c>
       <c r="D49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E49" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="I49">
-        <v>1500</v>
+        <v>95</v>
       </c>
       <c r="J49">
-        <v>2300</v>
+        <v>600</v>
       </c>
       <c r="K49" t="s">
         <v>37</v>
       </c>
-      <c r="L49" s="25" t="s">
-        <v>185</v>
-      </c>
-      <c r="N49" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="O49" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="P49" s="25" t="s">
-        <v>173</v>
+      <c r="M49" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
@@ -3246,31 +3258,22 @@
         <v>53</v>
       </c>
       <c r="D50" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E50" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="I50">
-        <v>1500</v>
+        <v>95</v>
       </c>
       <c r="J50">
-        <v>2300</v>
+        <v>600</v>
       </c>
       <c r="K50" t="s">
         <v>37</v>
       </c>
-      <c r="L50" s="25" t="s">
-        <v>185</v>
-      </c>
-      <c r="N50" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="O50" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="P50" s="25" t="s">
-        <v>173</v>
+      <c r="M50" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
@@ -3281,19 +3284,22 @@
         <v>53</v>
       </c>
       <c r="D51" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E51" t="s">
         <v>58</v>
       </c>
       <c r="I51">
-        <v>550</v>
+        <v>1500</v>
+      </c>
+      <c r="J51">
+        <v>2300</v>
       </c>
       <c r="K51" t="s">
         <v>37</v>
       </c>
       <c r="L51" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N51" s="25" t="s">
         <v>173</v>
@@ -3313,19 +3319,22 @@
         <v>53</v>
       </c>
       <c r="D52" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E52" t="s">
         <v>58</v>
       </c>
       <c r="I52">
-        <v>550</v>
+        <v>1500</v>
+      </c>
+      <c r="J52">
+        <v>2300</v>
       </c>
       <c r="K52" t="s">
         <v>37</v>
       </c>
       <c r="L52" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N52" s="25" t="s">
         <v>173</v>
@@ -3345,22 +3354,19 @@
         <v>53</v>
       </c>
       <c r="D53" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E53" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="I53">
-        <v>70</v>
-      </c>
-      <c r="J53">
-        <v>300</v>
+        <v>550</v>
       </c>
       <c r="K53" t="s">
         <v>37</v>
       </c>
       <c r="L53" s="25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="N53" s="25" t="s">
         <v>173</v>
@@ -3380,22 +3386,19 @@
         <v>53</v>
       </c>
       <c r="D54" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E54" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="I54">
-        <v>70</v>
-      </c>
-      <c r="J54">
-        <v>300</v>
+        <v>550</v>
       </c>
       <c r="K54" t="s">
         <v>37</v>
       </c>
       <c r="L54" s="25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="N54" s="25" t="s">
         <v>173</v>
@@ -3414,29 +3417,23 @@
       <c r="B55" t="s">
         <v>53</v>
       </c>
-      <c r="C55" t="s">
-        <v>91</v>
-      </c>
       <c r="D55" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E55" t="s">
-        <v>58</v>
-      </c>
-      <c r="G55">
-        <v>6.2</v>
-      </c>
-      <c r="H55">
-        <v>7.5</v>
+        <v>82</v>
+      </c>
+      <c r="I55">
+        <v>70</v>
       </c>
       <c r="J55">
-        <v>25</v>
+        <v>300</v>
       </c>
       <c r="K55" t="s">
         <v>37</v>
       </c>
       <c r="L55" s="25" t="s">
-        <v>228</v>
+        <v>188</v>
       </c>
       <c r="N55" s="25" t="s">
         <v>173</v>
@@ -3450,34 +3447,28 @@
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B56" t="s">
         <v>53</v>
       </c>
-      <c r="C56" t="s">
-        <v>93</v>
-      </c>
       <c r="D56" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E56" t="s">
-        <v>58</v>
-      </c>
-      <c r="G56">
-        <v>7.6</v>
-      </c>
-      <c r="H56">
-        <v>9.3000000000000007</v>
+        <v>82</v>
+      </c>
+      <c r="I56">
+        <v>70</v>
       </c>
       <c r="J56">
-        <v>25</v>
+        <v>300</v>
       </c>
       <c r="K56" t="s">
         <v>37</v>
       </c>
       <c r="L56" s="25" t="s">
-        <v>229</v>
+        <v>188</v>
       </c>
       <c r="N56" s="25" t="s">
         <v>173</v>
@@ -3497,7 +3488,7 @@
         <v>53</v>
       </c>
       <c r="C57" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D57" t="s">
         <v>92</v>
@@ -3506,10 +3497,10 @@
         <v>58</v>
       </c>
       <c r="G57">
-        <v>8.9</v>
+        <v>6.2</v>
       </c>
       <c r="H57">
-        <v>11</v>
+        <v>7.5</v>
       </c>
       <c r="J57">
         <v>25</v>
@@ -3518,7 +3509,7 @@
         <v>37</v>
       </c>
       <c r="L57" s="25" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="N57" s="25" t="s">
         <v>173</v>
@@ -3532,13 +3523,13 @@
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B58" t="s">
         <v>53</v>
       </c>
       <c r="C58" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D58" t="s">
         <v>92</v>
@@ -3547,10 +3538,10 @@
         <v>58</v>
       </c>
       <c r="G58">
-        <v>7.5</v>
+        <v>7.6</v>
       </c>
       <c r="H58">
-        <v>9.4</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="J58">
         <v>25</v>
@@ -3573,13 +3564,13 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B59" t="s">
         <v>53</v>
       </c>
       <c r="C59" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D59" t="s">
         <v>92</v>
@@ -3588,10 +3579,10 @@
         <v>58</v>
       </c>
       <c r="G59">
-        <v>9.3000000000000007</v>
+        <v>8.9</v>
       </c>
       <c r="H59">
-        <v>11.7</v>
+        <v>11</v>
       </c>
       <c r="J59">
         <v>25</v>
@@ -3620,7 +3611,7 @@
         <v>53</v>
       </c>
       <c r="C60" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D60" t="s">
         <v>92</v>
@@ -3629,10 +3620,10 @@
         <v>58</v>
       </c>
       <c r="G60">
-        <v>11</v>
+        <v>7.5</v>
       </c>
       <c r="H60">
-        <v>14</v>
+        <v>9.4</v>
       </c>
       <c r="J60">
         <v>25</v>
@@ -3641,7 +3632,7 @@
         <v>37</v>
       </c>
       <c r="L60" s="25" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="N60" s="25" t="s">
         <v>173</v>
@@ -3655,34 +3646,34 @@
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B61" t="s">
-        <v>95</v>
+        <v>53</v>
+      </c>
+      <c r="C61" t="s">
+        <v>93</v>
       </c>
       <c r="D61" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E61" t="s">
-        <v>55</v>
-      </c>
-      <c r="F61">
-        <v>4</v>
-      </c>
-      <c r="I61">
-        <v>10</v>
+        <v>58</v>
+      </c>
+      <c r="G61">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="H61">
+        <v>11.7</v>
       </c>
       <c r="J61">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="K61" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="L61" s="25" t="s">
-        <v>240</v>
-      </c>
-      <c r="M61" t="s">
-        <v>97</v>
+        <v>228</v>
       </c>
       <c r="N61" s="25" t="s">
         <v>173</v>
@@ -3690,48 +3681,54 @@
       <c r="O61" s="25" t="s">
         <v>173</v>
       </c>
-      <c r="P61" s="25"/>
+      <c r="P61" s="25" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B62" t="s">
-        <v>98</v>
+        <v>53</v>
+      </c>
+      <c r="C62" t="s">
+        <v>94</v>
       </c>
       <c r="D62" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E62" t="s">
-        <v>55</v>
-      </c>
-      <c r="F62">
-        <v>4</v>
-      </c>
-      <c r="I62">
-        <v>15</v>
+        <v>58</v>
+      </c>
+      <c r="G62">
+        <v>11</v>
+      </c>
+      <c r="H62">
+        <v>14</v>
       </c>
       <c r="J62">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="K62" t="s">
-        <v>99</v>
+        <v>37</v>
       </c>
       <c r="L62" s="25" t="s">
-        <v>240</v>
-      </c>
-      <c r="M62" t="s">
-        <v>100</v>
-      </c>
-      <c r="N62" s="25"/>
-      <c r="O62" s="25"/>
+        <v>229</v>
+      </c>
+      <c r="N62" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O62" s="25" t="s">
+        <v>173</v>
+      </c>
       <c r="P62" s="25" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B63" t="s">
         <v>95</v>
@@ -3755,7 +3752,7 @@
         <v>26</v>
       </c>
       <c r="L63" s="25" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M63" t="s">
         <v>97</v>
@@ -3770,7 +3767,7 @@
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B64" t="s">
         <v>98</v>
@@ -3794,7 +3791,7 @@
         <v>99</v>
       </c>
       <c r="L64" s="25" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M64" t="s">
         <v>100</v>
@@ -3807,7 +3804,7 @@
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B65" t="s">
         <v>95</v>
@@ -3815,18 +3812,23 @@
       <c r="D65" t="s">
         <v>96</v>
       </c>
-      <c r="E65" s="15" t="s">
-        <v>215</v>
-      </c>
-      <c r="F65" s="15"/>
+      <c r="E65" t="s">
+        <v>55</v>
+      </c>
+      <c r="F65">
+        <v>4</v>
+      </c>
       <c r="I65">
-        <v>0.83</v>
+        <v>10</v>
+      </c>
+      <c r="J65">
+        <v>20</v>
       </c>
       <c r="K65" t="s">
         <v>26</v>
       </c>
       <c r="L65" s="25" t="s">
-        <v>227</v>
+        <v>239</v>
       </c>
       <c r="M65" t="s">
         <v>97</v>
@@ -3841,7 +3843,7 @@
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B66" t="s">
         <v>98</v>
@@ -3849,18 +3851,23 @@
       <c r="D66" t="s">
         <v>96</v>
       </c>
-      <c r="E66" s="15" t="s">
-        <v>215</v>
-      </c>
-      <c r="F66" s="15"/>
+      <c r="E66" t="s">
+        <v>55</v>
+      </c>
+      <c r="F66">
+        <v>4</v>
+      </c>
       <c r="I66">
-        <v>1</v>
+        <v>15</v>
+      </c>
+      <c r="J66">
+        <v>20</v>
       </c>
       <c r="K66" t="s">
         <v>99</v>
       </c>
       <c r="L66" s="25" t="s">
-        <v>227</v>
+        <v>239</v>
       </c>
       <c r="M66" t="s">
         <v>100</v>
@@ -3873,7 +3880,7 @@
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B67" t="s">
         <v>95</v>
@@ -3882,7 +3889,7 @@
         <v>96</v>
       </c>
       <c r="E67" s="15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F67" s="15"/>
       <c r="I67">
@@ -3892,7 +3899,7 @@
         <v>26</v>
       </c>
       <c r="L67" s="25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M67" t="s">
         <v>97</v>
@@ -3907,7 +3914,7 @@
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B68" t="s">
         <v>98</v>
@@ -3916,7 +3923,7 @@
         <v>96</v>
       </c>
       <c r="E68" s="15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F68" s="15"/>
       <c r="I68">
@@ -3926,7 +3933,7 @@
         <v>99</v>
       </c>
       <c r="L68" s="25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M68" t="s">
         <v>100</v>
@@ -3939,50 +3946,68 @@
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B69" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D69" t="s">
-        <v>102</v>
-      </c>
-      <c r="E69" t="s">
-        <v>65</v>
-      </c>
-      <c r="J69">
-        <v>100</v>
+        <v>96</v>
+      </c>
+      <c r="E69" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="F69" s="15"/>
+      <c r="I69">
+        <v>0.83</v>
       </c>
       <c r="K69" t="s">
-        <v>30</v>
+        <v>26</v>
+      </c>
+      <c r="L69" s="25" t="s">
+        <v>226</v>
       </c>
       <c r="M69" t="s">
-        <v>75</v>
-      </c>
-      <c r="N69" s="25"/>
-      <c r="O69" s="25"/>
+        <v>97</v>
+      </c>
+      <c r="N69" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O69" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P69" s="25"/>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>56</v>
       </c>
       <c r="B70" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D70" t="s">
-        <v>102</v>
-      </c>
-      <c r="E70" t="s">
-        <v>65</v>
-      </c>
-      <c r="J70">
+        <v>96</v>
+      </c>
+      <c r="E70" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="F70" s="15"/>
+      <c r="I70">
+        <v>1</v>
+      </c>
+      <c r="K70" t="s">
+        <v>99</v>
+      </c>
+      <c r="L70" s="25" t="s">
+        <v>226</v>
+      </c>
+      <c r="M70" t="s">
         <v>100</v>
       </c>
-      <c r="K70" t="s">
-        <v>30</v>
-      </c>
-      <c r="M70" t="s">
-        <v>75</v>
+      <c r="N70" s="25"/>
+      <c r="O70" s="25"/>
+      <c r="P70" s="25" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
@@ -3992,33 +4017,23 @@
       <c r="B71" t="s">
         <v>101</v>
       </c>
-      <c r="D71" s="14" t="s">
-        <v>207</v>
-      </c>
-      <c r="E71" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="F71" s="14">
-        <v>4</v>
+      <c r="D71" t="s">
+        <v>102</v>
+      </c>
+      <c r="E71" t="s">
+        <v>65</v>
       </c>
       <c r="J71">
-        <v>0.1</v>
-      </c>
-      <c r="K71" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="L71" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="N71" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="O71" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="P71" s="25" t="s">
-        <v>173</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="K71" t="s">
+        <v>30</v>
+      </c>
+      <c r="M71" t="s">
+        <v>75</v>
+      </c>
+      <c r="N71" s="25"/>
+      <c r="O71" s="25"/>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
@@ -4027,32 +4042,20 @@
       <c r="B72" t="s">
         <v>101</v>
       </c>
-      <c r="D72" s="14" t="s">
-        <v>207</v>
-      </c>
-      <c r="E72" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="F72" s="14">
-        <v>4</v>
+      <c r="D72" t="s">
+        <v>102</v>
+      </c>
+      <c r="E72" t="s">
+        <v>65</v>
       </c>
       <c r="J72">
-        <v>0.1</v>
-      </c>
-      <c r="K72" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="L72" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="N72" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="O72" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="P72" s="25" t="s">
-        <v>173</v>
+        <v>100</v>
+      </c>
+      <c r="K72" t="s">
+        <v>30</v>
+      </c>
+      <c r="M72" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
@@ -4060,28 +4063,25 @@
         <v>52</v>
       </c>
       <c r="B73" t="s">
-        <v>53</v>
-      </c>
-      <c r="D73" t="s">
-        <v>103</v>
-      </c>
-      <c r="E73" t="s">
-        <v>104</v>
-      </c>
-      <c r="G73">
-        <v>490</v>
-      </c>
-      <c r="H73">
-        <v>650</v>
+        <v>101</v>
+      </c>
+      <c r="D73" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="E73" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F73" s="14">
+        <v>4</v>
       </c>
       <c r="J73">
-        <v>3000</v>
-      </c>
-      <c r="K73" t="s">
-        <v>37</v>
-      </c>
-      <c r="L73" s="10" t="s">
-        <v>189</v>
+        <v>10</v>
+      </c>
+      <c r="K73" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="L73" s="25" t="s">
+        <v>240</v>
       </c>
       <c r="N73" s="25" t="s">
         <v>173</v>
@@ -4098,28 +4098,25 @@
         <v>56</v>
       </c>
       <c r="B74" t="s">
-        <v>53</v>
-      </c>
-      <c r="D74" t="s">
-        <v>103</v>
-      </c>
-      <c r="E74" t="s">
-        <v>104</v>
-      </c>
-      <c r="G74">
-        <v>580</v>
-      </c>
-      <c r="H74">
-        <v>750</v>
+        <v>101</v>
+      </c>
+      <c r="D74" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="E74" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F74" s="14">
+        <v>4</v>
       </c>
       <c r="J74">
-        <v>3000</v>
-      </c>
-      <c r="K74" t="s">
-        <v>37</v>
-      </c>
-      <c r="L74" s="10" t="s">
-        <v>189</v>
+        <v>10</v>
+      </c>
+      <c r="K74" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="L74" s="25" t="s">
+        <v>240</v>
       </c>
       <c r="N74" s="25" t="s">
         <v>173</v>
@@ -4139,25 +4136,25 @@
         <v>53</v>
       </c>
       <c r="D75" t="s">
-        <v>105</v>
-      </c>
-      <c r="E75" s="25" t="s">
-        <v>226</v>
-      </c>
-      <c r="F75" s="14">
-        <v>1</v>
+        <v>103</v>
+      </c>
+      <c r="E75" t="s">
+        <v>104</v>
       </c>
       <c r="G75">
-        <v>3.0144442118484405E-4</v>
+        <v>490</v>
       </c>
       <c r="H75">
-        <v>4.1867280720117199E-4</v>
+        <v>650</v>
+      </c>
+      <c r="J75">
+        <v>3000</v>
       </c>
       <c r="K75" t="s">
         <v>37</v>
       </c>
-      <c r="L75" s="25" t="s">
-        <v>242</v>
+      <c r="L75" s="10" t="s">
+        <v>189</v>
       </c>
       <c r="N75" s="25" t="s">
         <v>173</v>
@@ -4177,25 +4174,25 @@
         <v>53</v>
       </c>
       <c r="D76" t="s">
-        <v>105</v>
-      </c>
-      <c r="E76" s="25" t="s">
-        <v>226</v>
-      </c>
-      <c r="F76" s="14">
-        <v>1</v>
+        <v>103</v>
+      </c>
+      <c r="E76" t="s">
+        <v>104</v>
       </c>
       <c r="G76">
-        <v>3.0144442118484405E-4</v>
+        <v>580</v>
       </c>
       <c r="H76">
-        <v>4.1867280720117231E-4</v>
+        <v>750</v>
+      </c>
+      <c r="J76">
+        <v>3000</v>
       </c>
       <c r="K76" t="s">
         <v>37</v>
       </c>
-      <c r="L76" s="25" t="s">
-        <v>242</v>
+      <c r="L76" s="10" t="s">
+        <v>189</v>
       </c>
       <c r="N76" s="25" t="s">
         <v>173</v>
@@ -4215,19 +4212,25 @@
         <v>53</v>
       </c>
       <c r="D77" t="s">
-        <v>106</v>
-      </c>
-      <c r="E77" t="s">
-        <v>82</v>
-      </c>
-      <c r="I77">
-        <v>4</v>
+        <v>105</v>
+      </c>
+      <c r="E77" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="F77" s="14">
+        <v>1</v>
+      </c>
+      <c r="G77">
+        <v>3.0144442118484405E-4</v>
+      </c>
+      <c r="H77">
+        <v>4.1867280720117199E-4</v>
       </c>
       <c r="K77" t="s">
         <v>37</v>
       </c>
       <c r="L77" s="25" t="s">
-        <v>191</v>
+        <v>241</v>
       </c>
       <c r="N77" s="25" t="s">
         <v>173</v>
@@ -4247,19 +4250,25 @@
         <v>53</v>
       </c>
       <c r="D78" t="s">
-        <v>106</v>
-      </c>
-      <c r="E78" t="s">
-        <v>82</v>
-      </c>
-      <c r="I78">
-        <v>4</v>
+        <v>105</v>
+      </c>
+      <c r="E78" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="F78" s="14">
+        <v>1</v>
+      </c>
+      <c r="G78">
+        <v>3.0144442118484405E-4</v>
+      </c>
+      <c r="H78">
+        <v>4.1867280720117231E-4</v>
       </c>
       <c r="K78" t="s">
         <v>37</v>
       </c>
       <c r="L78" s="25" t="s">
-        <v>191</v>
+        <v>241</v>
       </c>
       <c r="N78" s="25" t="s">
         <v>173</v>
@@ -4279,22 +4288,19 @@
         <v>53</v>
       </c>
       <c r="D79" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E79" t="s">
-        <v>58</v>
-      </c>
-      <c r="G79">
-        <v>1.3</v>
-      </c>
-      <c r="H79">
-        <v>1.6</v>
+        <v>82</v>
+      </c>
+      <c r="I79">
+        <v>4</v>
       </c>
       <c r="K79" t="s">
         <v>37</v>
       </c>
       <c r="L79" s="25" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N79" s="25" t="s">
         <v>173</v>
@@ -4314,22 +4320,19 @@
         <v>53</v>
       </c>
       <c r="D80" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E80" t="s">
-        <v>58</v>
-      </c>
-      <c r="G80">
-        <v>1.3</v>
-      </c>
-      <c r="H80">
-        <v>1.6</v>
+        <v>82</v>
+      </c>
+      <c r="I80">
+        <v>4</v>
       </c>
       <c r="K80" t="s">
         <v>37</v>
       </c>
       <c r="L80" s="25" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N80" s="25" t="s">
         <v>173</v>
@@ -4349,25 +4352,22 @@
         <v>53</v>
       </c>
       <c r="D81" t="s">
-        <v>108</v>
-      </c>
-      <c r="E81" s="25" t="s">
-        <v>226</v>
-      </c>
-      <c r="F81" s="14">
-        <v>1</v>
+        <v>107</v>
+      </c>
+      <c r="E81" t="s">
+        <v>58</v>
       </c>
       <c r="G81">
-        <v>5.4427464936152399E-3</v>
+        <v>1.3</v>
       </c>
       <c r="H81">
-        <v>6.698764915218757E-3</v>
+        <v>1.6</v>
       </c>
       <c r="K81" t="s">
         <v>37</v>
       </c>
       <c r="L81" s="25" t="s">
-        <v>243</v>
+        <v>192</v>
       </c>
       <c r="N81" s="25" t="s">
         <v>173</v>
@@ -4387,25 +4387,22 @@
         <v>53</v>
       </c>
       <c r="D82" t="s">
-        <v>108</v>
-      </c>
-      <c r="E82" s="25" t="s">
-        <v>226</v>
-      </c>
-      <c r="F82" s="14">
-        <v>1</v>
+        <v>107</v>
+      </c>
+      <c r="E82" t="s">
+        <v>58</v>
       </c>
       <c r="G82">
-        <v>5.4427464936152399E-3</v>
+        <v>1.3</v>
       </c>
       <c r="H82">
-        <v>6.698764915218757E-3</v>
+        <v>1.6</v>
       </c>
       <c r="K82" t="s">
         <v>37</v>
       </c>
       <c r="L82" s="25" t="s">
-        <v>243</v>
+        <v>192</v>
       </c>
       <c r="N82" s="25" t="s">
         <v>173</v>
@@ -4425,23 +4422,35 @@
         <v>53</v>
       </c>
       <c r="D83" t="s">
-        <v>109</v>
-      </c>
-      <c r="E83" t="s">
-        <v>58</v>
-      </c>
-      <c r="J83">
-        <v>10</v>
+        <v>108</v>
+      </c>
+      <c r="E83" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="F83" s="14">
+        <v>1</v>
+      </c>
+      <c r="G83">
+        <v>5.4427464936152399E-3</v>
+      </c>
+      <c r="H83">
+        <v>6.698764915218757E-3</v>
       </c>
       <c r="K83" t="s">
         <v>37</v>
       </c>
-      <c r="M83" t="s">
-        <v>75</v>
-      </c>
-      <c r="N83" s="25"/>
-      <c r="O83" s="25"/>
-      <c r="P83" s="25"/>
+      <c r="L83" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="N83" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O83" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P83" s="25" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
@@ -4451,23 +4460,35 @@
         <v>53</v>
       </c>
       <c r="D84" t="s">
-        <v>109</v>
-      </c>
-      <c r="E84" t="s">
-        <v>58</v>
-      </c>
-      <c r="J84">
-        <v>10</v>
+        <v>108</v>
+      </c>
+      <c r="E84" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="F84" s="14">
+        <v>1</v>
+      </c>
+      <c r="G84">
+        <v>5.4427464936152399E-3</v>
+      </c>
+      <c r="H84">
+        <v>6.698764915218757E-3</v>
       </c>
       <c r="K84" t="s">
         <v>37</v>
       </c>
-      <c r="M84" t="s">
-        <v>75</v>
-      </c>
-      <c r="N84" s="25"/>
-      <c r="O84" s="25"/>
-      <c r="P84" s="25"/>
+      <c r="L84" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="N84" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O84" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P84" s="25" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
@@ -4477,13 +4498,13 @@
         <v>53</v>
       </c>
       <c r="D85" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E85" t="s">
         <v>58</v>
       </c>
       <c r="J85">
-        <v>900</v>
+        <v>10</v>
       </c>
       <c r="K85" t="s">
         <v>37</v>
@@ -4491,6 +4512,9 @@
       <c r="M85" t="s">
         <v>75</v>
       </c>
+      <c r="N85" s="25"/>
+      <c r="O85" s="25"/>
+      <c r="P85" s="25"/>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
@@ -4500,13 +4524,13 @@
         <v>53</v>
       </c>
       <c r="D86" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E86" t="s">
         <v>58</v>
       </c>
       <c r="J86">
-        <v>900</v>
+        <v>10</v>
       </c>
       <c r="K86" t="s">
         <v>37</v>
@@ -4514,6 +4538,9 @@
       <c r="M86" t="s">
         <v>75</v>
       </c>
+      <c r="N86" s="25"/>
+      <c r="O86" s="25"/>
+      <c r="P86" s="25"/>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
@@ -4523,28 +4550,19 @@
         <v>53</v>
       </c>
       <c r="D87" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E87" t="s">
         <v>58</v>
       </c>
-      <c r="I87">
-        <v>5</v>
+      <c r="J87">
+        <v>900</v>
       </c>
       <c r="K87" t="s">
         <v>37</v>
       </c>
-      <c r="L87" s="25" t="s">
-        <v>193</v>
-      </c>
-      <c r="N87" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="O87" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="P87" s="25" t="s">
-        <v>173</v>
+      <c r="M87" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.25">
@@ -4555,28 +4573,19 @@
         <v>53</v>
       </c>
       <c r="D88" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E88" t="s">
         <v>58</v>
       </c>
-      <c r="I88">
-        <v>6</v>
+      <c r="J88">
+        <v>900</v>
       </c>
       <c r="K88" t="s">
         <v>37</v>
       </c>
-      <c r="L88" s="25" t="s">
-        <v>193</v>
-      </c>
-      <c r="N88" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="O88" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="P88" s="25" t="s">
-        <v>173</v>
+      <c r="M88" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.25">
@@ -4587,25 +4596,19 @@
         <v>53</v>
       </c>
       <c r="D89" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E89" t="s">
         <v>58</v>
       </c>
-      <c r="G89">
-        <v>1.5</v>
-      </c>
-      <c r="H89">
-        <v>1.6</v>
-      </c>
-      <c r="J89">
-        <v>25</v>
+      <c r="I89">
+        <v>5</v>
       </c>
       <c r="K89" t="s">
         <v>37</v>
       </c>
       <c r="L89" s="25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="N89" s="25" t="s">
         <v>173</v>
@@ -4625,25 +4628,19 @@
         <v>53</v>
       </c>
       <c r="D90" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E90" t="s">
         <v>58</v>
       </c>
-      <c r="G90">
-        <v>1.5</v>
-      </c>
-      <c r="H90">
-        <v>1.7</v>
-      </c>
-      <c r="J90">
-        <v>25</v>
+      <c r="I90">
+        <v>6</v>
       </c>
       <c r="K90" t="s">
         <v>37</v>
       </c>
       <c r="L90" s="25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="N90" s="25" t="s">
         <v>173</v>
@@ -4663,19 +4660,34 @@
         <v>53</v>
       </c>
       <c r="D91" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E91" t="s">
-        <v>82</v>
-      </c>
-      <c r="I91">
-        <v>40</v>
+        <v>58</v>
+      </c>
+      <c r="G91">
+        <v>1.5</v>
+      </c>
+      <c r="H91">
+        <v>1.6</v>
+      </c>
+      <c r="J91">
+        <v>25</v>
       </c>
       <c r="K91" t="s">
         <v>37</v>
       </c>
-      <c r="M91" t="s">
-        <v>75</v>
+      <c r="L91" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="N91" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O91" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P91" s="25" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.25">
@@ -4686,19 +4698,34 @@
         <v>53</v>
       </c>
       <c r="D92" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E92" t="s">
-        <v>82</v>
-      </c>
-      <c r="I92">
-        <v>40</v>
+        <v>58</v>
+      </c>
+      <c r="G92">
+        <v>1.5</v>
+      </c>
+      <c r="H92">
+        <v>1.7</v>
+      </c>
+      <c r="J92">
+        <v>25</v>
       </c>
       <c r="K92" t="s">
         <v>37</v>
       </c>
-      <c r="M92" t="s">
-        <v>75</v>
+      <c r="L92" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="N92" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O92" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P92" s="25" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.25">
@@ -4709,31 +4736,19 @@
         <v>53</v>
       </c>
       <c r="D93" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E93" t="s">
         <v>82</v>
       </c>
-      <c r="G93">
-        <v>250</v>
-      </c>
-      <c r="H93">
-        <v>330</v>
+      <c r="I93">
+        <v>40</v>
       </c>
       <c r="K93" t="s">
         <v>37</v>
       </c>
-      <c r="L93" s="25" t="s">
-        <v>195</v>
-      </c>
-      <c r="N93" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="O93" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="P93" s="25" t="s">
-        <v>173</v>
+      <c r="M93" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.25">
@@ -4744,31 +4759,19 @@
         <v>53</v>
       </c>
       <c r="D94" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E94" t="s">
         <v>82</v>
       </c>
-      <c r="G94">
-        <v>250</v>
-      </c>
-      <c r="H94">
-        <v>330</v>
+      <c r="I94">
+        <v>40</v>
       </c>
       <c r="K94" t="s">
         <v>37</v>
       </c>
-      <c r="L94" s="25" t="s">
-        <v>195</v>
-      </c>
-      <c r="N94" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="O94" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="P94" s="25" t="s">
-        <v>173</v>
+      <c r="M94" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.25">
@@ -4779,19 +4782,31 @@
         <v>53</v>
       </c>
       <c r="D95" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E95" t="s">
         <v>82</v>
       </c>
-      <c r="J95">
-        <v>1000</v>
+      <c r="G95">
+        <v>250</v>
+      </c>
+      <c r="H95">
+        <v>330</v>
       </c>
       <c r="K95" t="s">
         <v>37</v>
       </c>
-      <c r="M95" t="s">
-        <v>75</v>
+      <c r="L95" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="N95" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O95" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P95" s="25" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.25">
@@ -4802,19 +4817,31 @@
         <v>53</v>
       </c>
       <c r="D96" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E96" t="s">
         <v>82</v>
       </c>
-      <c r="J96">
-        <v>1000</v>
+      <c r="G96">
+        <v>250</v>
+      </c>
+      <c r="H96">
+        <v>330</v>
       </c>
       <c r="K96" t="s">
         <v>37</v>
       </c>
-      <c r="M96" t="s">
-        <v>75</v>
+      <c r="L96" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="N96" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O96" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P96" s="25" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.25">
@@ -4825,31 +4852,19 @@
         <v>53</v>
       </c>
       <c r="D97" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E97" t="s">
-        <v>58</v>
-      </c>
-      <c r="G97">
-        <v>90</v>
-      </c>
-      <c r="H97">
-        <v>110</v>
+        <v>82</v>
+      </c>
+      <c r="J97">
+        <v>1000</v>
       </c>
       <c r="K97" t="s">
         <v>37</v>
       </c>
-      <c r="L97" s="25" t="s">
-        <v>196</v>
-      </c>
-      <c r="N97" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="O97" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="P97" s="25" t="s">
-        <v>173</v>
+      <c r="M97" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.25">
@@ -4860,31 +4875,19 @@
         <v>53</v>
       </c>
       <c r="D98" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E98" t="s">
-        <v>58</v>
-      </c>
-      <c r="G98">
-        <v>90</v>
-      </c>
-      <c r="H98">
-        <v>110</v>
+        <v>82</v>
+      </c>
+      <c r="J98">
+        <v>1000</v>
       </c>
       <c r="K98" t="s">
         <v>37</v>
       </c>
-      <c r="L98" s="25" t="s">
-        <v>196</v>
-      </c>
-      <c r="N98" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="O98" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="P98" s="25" t="s">
-        <v>173</v>
+      <c r="M98" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.25">
@@ -4895,22 +4898,22 @@
         <v>53</v>
       </c>
       <c r="D99" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E99" t="s">
-        <v>82</v>
-      </c>
-      <c r="I99">
-        <v>15</v>
-      </c>
-      <c r="J99">
-        <v>100</v>
+        <v>58</v>
+      </c>
+      <c r="G99">
+        <v>90</v>
+      </c>
+      <c r="H99">
+        <v>110</v>
       </c>
       <c r="K99" t="s">
         <v>37</v>
       </c>
       <c r="L99" s="25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="N99" s="25" t="s">
         <v>173</v>
@@ -4930,22 +4933,22 @@
         <v>53</v>
       </c>
       <c r="D100" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E100" t="s">
-        <v>82</v>
-      </c>
-      <c r="I100">
-        <v>15</v>
-      </c>
-      <c r="J100">
-        <v>100</v>
+        <v>58</v>
+      </c>
+      <c r="G100">
+        <v>90</v>
+      </c>
+      <c r="H100">
+        <v>110</v>
       </c>
       <c r="K100" t="s">
         <v>37</v>
       </c>
       <c r="L100" s="25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="N100" s="25" t="s">
         <v>173</v>
@@ -4965,19 +4968,22 @@
         <v>53</v>
       </c>
       <c r="D101" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E101" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="I101">
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="J101">
+        <v>100</v>
       </c>
       <c r="K101" t="s">
         <v>37</v>
       </c>
       <c r="L101" s="25" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="N101" s="25" t="s">
         <v>173</v>
@@ -4997,19 +5003,22 @@
         <v>53</v>
       </c>
       <c r="D102" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E102" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="I102">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="J102">
+        <v>100</v>
       </c>
       <c r="K102" t="s">
         <v>37</v>
       </c>
       <c r="L102" s="25" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="N102" s="25" t="s">
         <v>173</v>
@@ -5029,19 +5038,28 @@
         <v>53</v>
       </c>
       <c r="D103" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E103" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="I103">
-        <v>79</v>
+        <v>9</v>
       </c>
       <c r="K103" t="s">
         <v>37</v>
       </c>
-      <c r="M103" s="6" t="s">
-        <v>120</v>
+      <c r="L103" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="N103" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O103" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P103" s="25" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.25">
@@ -5052,19 +5070,28 @@
         <v>53</v>
       </c>
       <c r="D104" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E104" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="I104">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="K104" t="s">
         <v>37</v>
       </c>
-      <c r="M104" s="6" t="s">
-        <v>120</v>
+      <c r="L104" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="N104" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O104" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="P104" s="25" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.25">
@@ -5075,19 +5102,19 @@
         <v>53</v>
       </c>
       <c r="D105" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E105" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="I105">
-        <v>400</v>
+        <v>79</v>
       </c>
       <c r="K105" t="s">
         <v>37</v>
       </c>
-      <c r="M105" t="s">
-        <v>75</v>
+      <c r="M105" s="6" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.25">
@@ -5098,23 +5125,69 @@
         <v>53</v>
       </c>
       <c r="D106" t="s">
+        <v>119</v>
+      </c>
+      <c r="E106" t="s">
+        <v>82</v>
+      </c>
+      <c r="I106">
+        <v>79</v>
+      </c>
+      <c r="K106" t="s">
+        <v>37</v>
+      </c>
+      <c r="M106" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>52</v>
+      </c>
+      <c r="B107" t="s">
+        <v>53</v>
+      </c>
+      <c r="D107" t="s">
         <v>121</v>
       </c>
-      <c r="E106" t="s">
-        <v>58</v>
-      </c>
-      <c r="I106">
+      <c r="E107" t="s">
+        <v>58</v>
+      </c>
+      <c r="I107">
         <v>400</v>
       </c>
-      <c r="K106" t="s">
-        <v>37</v>
-      </c>
-      <c r="M106" t="s">
+      <c r="K107" t="s">
+        <v>37</v>
+      </c>
+      <c r="M107" t="s">
         <v>75</v>
       </c>
     </row>
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>56</v>
+      </c>
+      <c r="B108" t="s">
+        <v>53</v>
+      </c>
+      <c r="D108" t="s">
+        <v>121</v>
+      </c>
+      <c r="E108" t="s">
+        <v>58</v>
+      </c>
+      <c r="I108">
+        <v>400</v>
+      </c>
+      <c r="K108" t="s">
+        <v>37</v>
+      </c>
+      <c r="M108" t="s">
+        <v>75</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:M106" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:M108" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
@@ -5124,12 +5197,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S507"/>
   <sheetViews>
-    <sheetView zoomScale="110" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E19" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D1" sqref="D1:D1048576"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A20" sqref="A20:XFD23"/>
+      <selection pane="bottomRight" activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5169,7 +5242,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="21" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L1" t="s">
         <v>50</v>
@@ -5212,14 +5285,32 @@
       <c r="F2">
         <v>9</v>
       </c>
+      <c r="J2">
+        <v>12</v>
+      </c>
       <c r="L2" t="s">
         <v>22</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="N2" s="14" t="s">
-        <v>213</v>
+        <v>232</v>
+      </c>
+      <c r="N2" s="28" t="s">
+        <v>244</v>
+      </c>
+      <c r="O2" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="P2" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q2" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="R2" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="S2" s="28" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -5238,14 +5329,32 @@
       <c r="F3">
         <v>9</v>
       </c>
+      <c r="J3">
+        <v>12</v>
+      </c>
       <c r="L3" t="s">
         <v>22</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="N3" t="s">
-        <v>122</v>
+        <v>232</v>
+      </c>
+      <c r="N3" s="28" t="s">
+        <v>244</v>
+      </c>
+      <c r="O3" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="P3" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q3" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="R3" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="S3" s="28" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -5256,7 +5365,7 @@
         <v>123</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E4" t="s">
         <v>58</v>
@@ -5265,7 +5374,7 @@
         <v>22</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N4" s="24"/>
     </row>
@@ -5277,7 +5386,7 @@
         <v>123</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E5" t="s">
         <v>58</v>
@@ -5286,7 +5395,7 @@
         <v>22</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N5" s="24"/>
     </row>
@@ -5298,7 +5407,7 @@
         <v>124</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E6" t="s">
         <v>58</v>
@@ -5307,7 +5416,7 @@
         <v>22</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N6" s="24"/>
       <c r="O6" s="8" t="s">
@@ -5322,7 +5431,7 @@
         <v>124</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E7" t="s">
         <v>58</v>
@@ -5331,7 +5440,7 @@
         <v>22</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N7" s="24"/>
       <c r="O7" s="8" t="s">
@@ -5346,7 +5455,7 @@
         <v>125</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E8" t="s">
         <v>58</v>
@@ -5355,7 +5464,7 @@
         <v>22</v>
       </c>
       <c r="M8" s="11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N8" s="24"/>
       <c r="P8" s="8" t="s">
@@ -5373,7 +5482,7 @@
         <v>125</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E9" t="s">
         <v>58</v>
@@ -5382,7 +5491,7 @@
         <v>22</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N9" s="24"/>
       <c r="P9" s="8" t="s">
@@ -5400,7 +5509,7 @@
         <v>126</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E10" t="s">
         <v>58</v>
@@ -5409,7 +5518,7 @@
         <v>22</v>
       </c>
       <c r="M10" s="11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N10" s="24"/>
       <c r="R10" s="8" t="s">
@@ -5427,7 +5536,7 @@
         <v>126</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E11" t="s">
         <v>58</v>
@@ -5436,7 +5545,7 @@
         <v>22</v>
       </c>
       <c r="M11" s="11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N11" s="24"/>
       <c r="R11" s="8" t="s">
@@ -5677,7 +5786,7 @@
         <v>22</v>
       </c>
       <c r="M20" s="20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
@@ -5697,7 +5806,7 @@
         <v>22</v>
       </c>
       <c r="M21" s="20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
@@ -5717,7 +5826,7 @@
         <v>22</v>
       </c>
       <c r="M22" s="20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
@@ -5737,7 +5846,7 @@
         <v>22</v>
       </c>
       <c r="M23" s="20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
@@ -5760,7 +5869,7 @@
         <v>22</v>
       </c>
       <c r="M24" s="20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="P24" s="8" t="s">
         <v>173</v>
@@ -5789,7 +5898,7 @@
         <v>22</v>
       </c>
       <c r="M25" s="20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="P25" s="8" t="s">
         <v>173</v>
@@ -5818,7 +5927,7 @@
         <v>22</v>
       </c>
       <c r="M26" s="20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="R26" s="8" t="s">
         <v>173</v>
@@ -5847,7 +5956,7 @@
         <v>22</v>
       </c>
       <c r="M27" s="20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="R27" s="8" t="s">
         <v>173</v>
@@ -5876,7 +5985,7 @@
         <v>22</v>
       </c>
       <c r="M28" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="N28" t="s">
         <v>122</v>
@@ -5902,7 +6011,7 @@
         <v>22</v>
       </c>
       <c r="M29" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="N29" t="s">
         <v>122</v>
@@ -5931,7 +6040,7 @@
         <v>22</v>
       </c>
       <c r="M30" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
@@ -5957,7 +6066,7 @@
         <v>22</v>
       </c>
       <c r="M31" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
@@ -5983,7 +6092,7 @@
         <v>22</v>
       </c>
       <c r="M32" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="O32" s="8" t="s">
         <v>173</v>
@@ -6012,7 +6121,7 @@
         <v>22</v>
       </c>
       <c r="M33" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="O33" s="8" t="s">
         <v>173</v>
@@ -6041,7 +6150,7 @@
         <v>22</v>
       </c>
       <c r="M34" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="P34" s="8" t="s">
         <v>173</v>
@@ -6073,7 +6182,7 @@
         <v>22</v>
       </c>
       <c r="M35" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="P35" s="8" t="s">
         <v>173</v>
@@ -6105,7 +6214,7 @@
         <v>22</v>
       </c>
       <c r="M36" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="R36" s="8" t="s">
         <v>173</v>
@@ -6137,7 +6246,7 @@
         <v>22</v>
       </c>
       <c r="M37" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="R37" s="8" t="s">
         <v>173</v>
@@ -6169,7 +6278,7 @@
         <v>22</v>
       </c>
       <c r="M38" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
@@ -6195,7 +6304,7 @@
         <v>22</v>
       </c>
       <c r="M39" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
@@ -6221,7 +6330,7 @@
         <v>22</v>
       </c>
       <c r="M40" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="O40" s="8" t="s">
         <v>173</v>
@@ -6250,7 +6359,7 @@
         <v>22</v>
       </c>
       <c r="M41" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="O41" s="8" t="s">
         <v>173</v>
@@ -6279,7 +6388,7 @@
         <v>22</v>
       </c>
       <c r="M42" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="P42" s="8" t="s">
         <v>173</v>
@@ -6311,7 +6420,7 @@
         <v>22</v>
       </c>
       <c r="M43" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="P43" s="8" t="s">
         <v>173</v>
@@ -6343,7 +6452,7 @@
         <v>22</v>
       </c>
       <c r="M44" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="R44" s="8" t="s">
         <v>173</v>
@@ -6375,7 +6484,7 @@
         <v>22</v>
       </c>
       <c r="M45" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="R45" s="8" t="s">
         <v>173</v>
@@ -6404,7 +6513,7 @@
         <v>22</v>
       </c>
       <c r="M46" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="N46" t="s">
         <v>122</v>
@@ -6430,7 +6539,7 @@
         <v>22</v>
       </c>
       <c r="M47" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="N47" t="s">
         <v>122</v>
@@ -6720,7 +6829,7 @@
         <v>203</v>
       </c>
       <c r="M58" s="11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="N58" s="14" t="s">
         <v>205</v>
@@ -6764,7 +6873,7 @@
         <v>203</v>
       </c>
       <c r="M59" s="11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="N59" s="14" t="s">
         <v>205</v>
@@ -6811,7 +6920,7 @@
         <v>26</v>
       </c>
       <c r="M60" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="O60" s="10" t="s">
         <v>173</v>
@@ -6843,7 +6952,7 @@
         <v>26</v>
       </c>
       <c r="M61" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N61" s="10" t="s">
         <v>199</v>
@@ -6880,7 +6989,7 @@
         <v>26</v>
       </c>
       <c r="M62" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N62" s="10" t="s">
         <v>199</v>
@@ -6917,7 +7026,7 @@
         <v>26</v>
       </c>
       <c r="M63" s="18" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N63" s="10" t="s">
         <v>199</v>
@@ -6955,7 +7064,7 @@
         <v>26</v>
       </c>
       <c r="M64" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="R64" s="8"/>
       <c r="S64" s="8" t="s">
@@ -6988,7 +7097,7 @@
         <v>26</v>
       </c>
       <c r="M65" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="O65" s="10" t="s">
         <v>173</v>
@@ -7020,7 +7129,7 @@
         <v>26</v>
       </c>
       <c r="M66" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N66" s="10" t="s">
         <v>199</v>
@@ -7057,7 +7166,7 @@
         <v>26</v>
       </c>
       <c r="M67" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N67" s="10" t="s">
         <v>199</v>
@@ -7094,7 +7203,7 @@
         <v>26</v>
       </c>
       <c r="M68" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N68" s="10" t="s">
         <v>199</v>
@@ -7132,7 +7241,7 @@
         <v>26</v>
       </c>
       <c r="M69" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="R69" s="8"/>
       <c r="S69" s="8" t="s">
@@ -7165,7 +7274,7 @@
         <v>22</v>
       </c>
       <c r="M70" s="11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O70" s="10" t="s">
         <v>173</v>
@@ -7197,7 +7306,7 @@
         <v>22</v>
       </c>
       <c r="M71" s="11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N71" s="10" t="s">
         <v>199</v>
@@ -7234,7 +7343,7 @@
         <v>22</v>
       </c>
       <c r="M72" s="11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N72" s="10" t="s">
         <v>199</v>
@@ -7271,7 +7380,7 @@
         <v>22</v>
       </c>
       <c r="M73" s="11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N73" s="10" t="s">
         <v>199</v>
@@ -7309,7 +7418,7 @@
         <v>22</v>
       </c>
       <c r="M74" s="11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O74" s="10" t="s">
         <v>173</v>
@@ -7341,7 +7450,7 @@
         <v>22</v>
       </c>
       <c r="M75" s="11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N75" s="10" t="s">
         <v>199</v>
@@ -7378,7 +7487,7 @@
         <v>22</v>
       </c>
       <c r="M76" s="11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N76" s="10" t="s">
         <v>199</v>
@@ -7415,7 +7524,7 @@
         <v>22</v>
       </c>
       <c r="M77" s="11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N77" s="10" t="s">
         <v>199</v>
@@ -8944,7 +9053,7 @@
         <v>37</v>
       </c>
       <c r="M136" s="25" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="137" spans="1:19" x14ac:dyDescent="0.25">
@@ -8970,7 +9079,7 @@
         <v>37</v>
       </c>
       <c r="M137" s="25" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="138" spans="1:19" x14ac:dyDescent="0.25">
@@ -8996,7 +9105,7 @@
         <v>37</v>
       </c>
       <c r="M138" s="25" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="O138" s="22" t="s">
         <v>173</v>
@@ -9025,7 +9134,7 @@
         <v>37</v>
       </c>
       <c r="M139" s="25" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="O139" s="22" t="s">
         <v>173</v>
@@ -9054,7 +9163,7 @@
         <v>37</v>
       </c>
       <c r="M140" s="25" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P140" s="22" t="s">
         <v>173</v>
@@ -9083,7 +9192,7 @@
         <v>37</v>
       </c>
       <c r="M141" s="25" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P141" s="22" t="s">
         <v>173</v>
@@ -9112,7 +9221,7 @@
         <v>37</v>
       </c>
       <c r="M142" s="25" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q142" s="22" t="s">
         <v>173</v>
@@ -9141,7 +9250,7 @@
         <v>37</v>
       </c>
       <c r="M143" s="25" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q143" s="22" t="s">
         <v>173</v>
@@ -9173,7 +9282,7 @@
         <v>37</v>
       </c>
       <c r="M144" s="25" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="R144" s="22" t="s">
         <v>173</v>
@@ -9208,7 +9317,7 @@
         <v>37</v>
       </c>
       <c r="M145" s="25" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="R145" s="22" t="s">
         <v>173</v>
@@ -9240,7 +9349,7 @@
         <v>37</v>
       </c>
       <c r="M146" s="25" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="R146" s="22" t="s">
         <v>173</v>
@@ -12660,7 +12769,7 @@
         <v>96</v>
       </c>
       <c r="E274" s="15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F274" s="15"/>
       <c r="G274" s="15">
@@ -12673,10 +12782,10 @@
       <c r="J274" s="15"/>
       <c r="K274" s="15"/>
       <c r="L274" s="15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="M274" s="25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N274" s="15"/>
       <c r="O274" s="15" t="s">
@@ -12699,7 +12808,7 @@
         <v>96</v>
       </c>
       <c r="E275" s="16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F275" s="15"/>
       <c r="G275" s="15">
@@ -12712,10 +12821,10 @@
       <c r="J275" s="15"/>
       <c r="K275" s="15"/>
       <c r="L275" s="15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="M275" s="25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N275" s="15"/>
       <c r="O275" s="15"/>
@@ -12731,14 +12840,14 @@
         <v>52</v>
       </c>
       <c r="B276" s="15" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C276" s="15"/>
       <c r="D276" s="15" t="s">
         <v>96</v>
       </c>
       <c r="E276" s="15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F276" s="15"/>
       <c r="G276" s="15">
@@ -12751,10 +12860,10 @@
       <c r="J276" s="15"/>
       <c r="K276" s="15"/>
       <c r="L276" s="15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="M276" s="25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N276" s="15"/>
       <c r="O276" s="15"/>
@@ -12777,7 +12886,7 @@
         <v>96</v>
       </c>
       <c r="E277" s="15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F277" s="15"/>
       <c r="G277" s="15">
@@ -12790,10 +12899,10 @@
       <c r="J277" s="15"/>
       <c r="K277" s="15"/>
       <c r="L277" s="15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="M277" s="25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N277" s="15"/>
       <c r="O277" s="15"/>
@@ -12816,7 +12925,7 @@
         <v>96</v>
       </c>
       <c r="E278" s="15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F278" s="15"/>
       <c r="G278" s="15">
@@ -12829,10 +12938,10 @@
       <c r="J278" s="15"/>
       <c r="K278" s="15"/>
       <c r="L278" s="15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="M278" s="25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N278" s="15"/>
       <c r="O278" s="15"/>
@@ -12855,7 +12964,7 @@
         <v>96</v>
       </c>
       <c r="E279" s="15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F279" s="15"/>
       <c r="G279" s="15">
@@ -12868,10 +12977,10 @@
       <c r="J279" s="15"/>
       <c r="K279" s="15"/>
       <c r="L279" s="15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="M279" s="25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N279" s="15"/>
       <c r="O279" s="15" t="s">
@@ -12894,7 +13003,7 @@
         <v>96</v>
       </c>
       <c r="E280" s="15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F280" s="15"/>
       <c r="G280" s="15">
@@ -12907,10 +13016,10 @@
       <c r="J280" s="15"/>
       <c r="K280" s="15"/>
       <c r="L280" s="15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="M280" s="25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N280" s="15"/>
       <c r="O280" s="15"/>
@@ -12926,14 +13035,14 @@
         <v>56</v>
       </c>
       <c r="B281" s="15" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C281" s="15"/>
       <c r="D281" s="15" t="s">
         <v>96</v>
       </c>
       <c r="E281" s="15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F281" s="15"/>
       <c r="G281" s="15">
@@ -12946,10 +13055,10 @@
       <c r="J281" s="15"/>
       <c r="K281" s="15"/>
       <c r="L281" s="15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="M281" s="25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N281" s="15"/>
       <c r="O281" s="15"/>
@@ -12972,7 +13081,7 @@
         <v>96</v>
       </c>
       <c r="E282" s="15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F282" s="15"/>
       <c r="G282" s="15">
@@ -12985,10 +13094,10 @@
       <c r="J282" s="15"/>
       <c r="K282" s="15"/>
       <c r="L282" s="15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="M282" s="25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N282" s="15"/>
       <c r="O282" s="15"/>
@@ -13011,7 +13120,7 @@
         <v>96</v>
       </c>
       <c r="E283" s="15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F283" s="15"/>
       <c r="G283" s="15">
@@ -13024,10 +13133,10 @@
       <c r="J283" s="15"/>
       <c r="K283" s="15"/>
       <c r="L283" s="15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="M283" s="25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N283" s="15"/>
       <c r="O283" s="15"/>
@@ -13064,7 +13173,7 @@
         <v>26</v>
       </c>
       <c r="M284" s="25" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="285" spans="1:19" x14ac:dyDescent="0.25">
@@ -13093,7 +13202,7 @@
         <v>26</v>
       </c>
       <c r="M285" s="25" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="O285" t="s">
         <v>173</v>
@@ -13128,7 +13237,7 @@
         <v>26</v>
       </c>
       <c r="M286" s="25" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="Q286" t="s">
         <v>173</v>
@@ -13160,7 +13269,7 @@
         <v>26</v>
       </c>
       <c r="M287" s="25" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="R287" t="s">
         <v>173</v>
@@ -13192,7 +13301,7 @@
         <v>26</v>
       </c>
       <c r="M288" s="25" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="S288" t="s">
         <v>173</v>
@@ -13224,7 +13333,7 @@
         <v>26</v>
       </c>
       <c r="M289" s="25" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="290" spans="1:19" x14ac:dyDescent="0.25">
@@ -13253,7 +13362,7 @@
         <v>26</v>
       </c>
       <c r="M290" s="25" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="O290" t="s">
         <v>173</v>
@@ -13288,7 +13397,7 @@
         <v>26</v>
       </c>
       <c r="M291" s="25" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="Q291" t="s">
         <v>173</v>
@@ -13320,7 +13429,7 @@
         <v>26</v>
       </c>
       <c r="M292" s="25" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="R292" t="s">
         <v>173</v>
@@ -13352,7 +13461,7 @@
         <v>26</v>
       </c>
       <c r="M293" s="25" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="S293" t="s">
         <v>173</v>
@@ -13421,7 +13530,7 @@
         <v>208</v>
       </c>
       <c r="M296" s="25" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="O296" s="14" t="s">
         <v>173</v>
@@ -13462,7 +13571,7 @@
         <v>208</v>
       </c>
       <c r="M297" s="25" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="O297" s="14" t="s">
         <v>173</v>
@@ -13971,7 +14080,7 @@
         <v>37</v>
       </c>
       <c r="M314" s="25" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="O314" s="23" t="s">
         <v>173</v>
@@ -14016,7 +14125,7 @@
         <v>37</v>
       </c>
       <c r="M315" s="25" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="O315" s="23" t="s">
         <v>173</v>
@@ -14840,7 +14949,7 @@
         <v>37</v>
       </c>
       <c r="M346" s="25" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="O346" s="10" t="s">
         <v>173</v>
@@ -14884,7 +14993,7 @@
         <v>37</v>
       </c>
       <c r="M347" s="25" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="O347" s="10" t="s">
         <v>173</v>
@@ -18866,7 +18975,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:S507" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
-  <phoneticPr fontId="22" type="noConversion"/>
+  <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>

</xml_diff>